<commit_message>
Updated table with initiatives included
</commit_message>
<xml_diff>
--- a/dat/synchros-initiatives.xlsx
+++ b/dat/synchros-initiatives.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mori.P16\Documents\Workspace\mapping-initiatives\dat\"/>
     </mc:Choice>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="3" r:id="rId1"/>
+    <sheet name="Table 1 updated" r:id="rId5" sheetId="4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="760">
   <si>
     <t>A consortium of agricultural cohort studies</t>
   </si>
@@ -1350,12 +1351,1020 @@
   </si>
   <si>
     <t>Adult Europeans</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>acronym</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>methodology.nbCohorts.total</t>
+  </si>
+  <si>
+    <t>methodology.nbCohorts.harmonized</t>
+  </si>
+  <si>
+    <t>methodology.moreCohortsToBeHarmonized</t>
+  </si>
+  <si>
+    <t>nbParticipants.total</t>
+  </si>
+  <si>
+    <t>nbParticipants.harmonized</t>
+  </si>
+  <si>
+    <t>age.min</t>
+  </si>
+  <si>
+    <t>age.max</t>
+  </si>
+  <si>
+    <t>methodology.nbHarmonizedVariables</t>
+  </si>
+  <si>
+    <t>cohortCriteria</t>
+  </si>
+  <si>
+    <t>countries</t>
+  </si>
+  <si>
+    <t>n_countries</t>
+  </si>
+  <si>
+    <t>age_range</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>BBMRI-NL</t>
+  </si>
+  <si>
+    <t>CanPath</t>
+  </si>
+  <si>
+    <t>CORDELIA</t>
+  </si>
+  <si>
+    <t>EClipSE</t>
+  </si>
+  <si>
+    <t>EPHOR</t>
+  </si>
+  <si>
+    <t>EPOSA</t>
+  </si>
+  <si>
+    <t>EUCAN-Connect</t>
+  </si>
+  <si>
+    <t>Gateway</t>
+  </si>
+  <si>
+    <t>HALCyon</t>
+  </si>
+  <si>
+    <t>HeLTI</t>
+  </si>
+  <si>
+    <t>I4C</t>
+  </si>
+  <si>
+    <t>ICC-dementia</t>
+  </si>
+  <si>
+    <t>IDEAR</t>
+  </si>
+  <si>
+    <t>IHCC</t>
+  </si>
+  <si>
+    <t>interconnect</t>
+  </si>
+  <si>
+    <t>InterLACE</t>
+  </si>
+  <si>
+    <t>LIFEPATH</t>
+  </si>
+  <si>
+    <t>OMEGA-NET</t>
+  </si>
+  <si>
+    <t>ReACH</t>
+  </si>
+  <si>
+    <t>SAPRIN</t>
+  </si>
+  <si>
+    <t>SIC</t>
+  </si>
+  <si>
+    <t>KoGES</t>
+  </si>
+  <si>
+    <t>RAND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Asia Cohort Consortium </t>
+  </si>
+  <si>
+    <t>CHANCES</t>
+  </si>
+  <si>
+    <t>ECHO</t>
+  </si>
+  <si>
+    <t>FinnGen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genome Asia 100K  </t>
+  </si>
+  <si>
+    <t>DEMETRIQ</t>
+  </si>
+  <si>
+    <t>Tohoku Medical Megabank Project</t>
+  </si>
+  <si>
+    <t>SAGE+</t>
+  </si>
+  <si>
+    <t>RECAP</t>
+  </si>
+  <si>
+    <t>CHICOS</t>
+  </si>
+  <si>
+    <t>LONGITOOLS</t>
+  </si>
+  <si>
+    <t>MeDALL</t>
+  </si>
+  <si>
+    <t>DYNOPTA</t>
+  </si>
+  <si>
+    <t>HAVIC</t>
+  </si>
+  <si>
+    <t>CHARGE</t>
+  </si>
+  <si>
+    <t>CAPICE</t>
+  </si>
+  <si>
+    <t>LIFESPAN</t>
+  </si>
+  <si>
+    <t>STOP</t>
+  </si>
+  <si>
+    <t>DYNAHEALTH</t>
+  </si>
+  <si>
+    <t>Ageing Trajectories of Health: Longitudinal Opportunities and Synergies</t>
+  </si>
+  <si>
+    <t>Biobank Standardisation and Harmonisation for Research Excellence in the European Union</t>
+  </si>
+  <si>
+    <t>Canadian Partnership for Tomorrow’s Health</t>
+  </si>
+  <si>
+    <t>Swedish Cohort Consortium</t>
+  </si>
+  <si>
+    <t>Collaborative cOhorts Reassembled Data to study mEchanisms and Longterm Incidence of chronic diseAses</t>
+  </si>
+  <si>
+    <t>Epidemiological  Clinicopathological Studies in Europe</t>
+  </si>
+  <si>
+    <t>Exposome Project for Health and Occupational Research</t>
+  </si>
+  <si>
+    <t>European Project on Osteoarthritis</t>
+  </si>
+  <si>
+    <t>The Gateway to Global Aging Data</t>
+  </si>
+  <si>
+    <t>Healthy Ageing  across the Life Course</t>
+  </si>
+  <si>
+    <t>The Human Early-Life Exposome</t>
+  </si>
+  <si>
+    <t>Healthy Life Trajectories Initiative</t>
+  </si>
+  <si>
+    <t>International Childhood Cardiovascular Cohort Consortium</t>
+  </si>
+  <si>
+    <t>International Childhood  Cancer Cohort Consortium</t>
+  </si>
+  <si>
+    <t>International  Centenarian Consortium - dementia</t>
+  </si>
+  <si>
+    <t>Integrated Datasets in Europe for Ageing Research</t>
+  </si>
+  <si>
+    <t>Interplay of Genes and Environment across Multiple Studies</t>
+  </si>
+  <si>
+    <t>International HundredK+ Cohorts Consortium</t>
+  </si>
+  <si>
+    <t>International Collaboration for a Life Course Approach to  Reproductive Health and Chronic Disease Events</t>
+  </si>
+  <si>
+    <t>Promoting mental well-being and healthy ageing in cities</t>
+  </si>
+  <si>
+    <t>National E-lnfrastructure for Aging Research</t>
+  </si>
+  <si>
+    <t>Network on the Coordination and Harmonisation of European Occupational Cohorts project</t>
+  </si>
+  <si>
+    <t>Research Advancement through Cohort Cataloguing and Harmonization</t>
+  </si>
+  <si>
+    <t>South African Population  Research Infrastructure Network</t>
+  </si>
+  <si>
+    <t>Social Inequality in Cancer cohort study</t>
+  </si>
+  <si>
+    <t>The Korean Genome and Epidemiology Study (KoGES) Consortium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEPREP    </t>
+  </si>
+  <si>
+    <t>CLOSER (Cohort and Longitudinal Studies Enhancement Resources)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPIRIT (Sino-Quebec Perinatal Initiative in Research and Information Technology)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consortium on Health and Ageing: Network of cohorts in Europe and the United States (CHANCES)    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environmental influences on Child Health Outcomes (ECHO): ECHO-wide Cohort    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finnish Genome Project (FinnGen) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEMETRIQ (Developing methodologies to reduce inequalities in the determinants of health)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAGE+ Wave 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research on European Children and adults born preterm (RECAP)  </t>
+  </si>
+  <si>
+    <t>DYNOPTA: Dynamic Analyses to Optimise Ageing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Hand-Arm Vibration International Consortium (HAVIC): Prospective Studies on the Relationship Between Power Tool Exposure and Health Effects     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHARGE Consortium </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIFESPAN (Early-life influences on suicidal ideation, suicide attempts and suicide mortality: a life-course perspective to inform prevention)        </t>
+  </si>
+  <si>
+    <t>Europe; Canada; Australia</t>
+  </si>
+  <si>
+    <t>America, Asia, Europe</t>
+  </si>
+  <si>
+    <t>America, Asia, Europe and Oceania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 countries from all over the world </t>
+  </si>
+  <si>
+    <t>Principally Canada</t>
+  </si>
+  <si>
+    <t>American, European, Asian countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Europe (27 countries)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Europe  </t>
+  </si>
+  <si>
+    <t>Australia, 15 European countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USA, Europe </t>
+  </si>
+  <si>
+    <t>The objective of AGRICOH is to support and mantain collaboration and data sharing/pooling to research the association between agricultural exposures and different health outcomes, with emphasis on associations that involve rare exposures and/or health outcomes, and for which data pooling represents a significant gain in statistical power compared to analysis of individual cohorts.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The objective of the ATHLOS Project is to achieve a better understanding of ageing by identifying patterns of healthy ageing pathways or trajectories, the determinants of those patterns, the critical points in time when changes in trajectories are produced, and to propose timely clinical and public health interventions to optimize healthy ageing. Moreover, a new definition of 'old age' based on many characteristics rather than just the classical chronological definition of age will be used for calculating projections in each specific population and guide policy recommendations. To do so, the Consortium will create a harmonised dataset with over 400,000 individuals collated from existing longitudinal studies of ageing and including information on physical and mental health, biomarkers, life style habits, social environment and participation, among others.&lt;/p&gt;
+&lt;p&gt;ATHLOS is a five-year project funded by the European Union's Horizon 2020 Research and Innovation Programme under grant agreement number 635316.&lt;/p&gt;
+&lt;p&gt;The Consortium is coordinated by Dr Josep Maria Haro (Parc Sanitari Sant Joan de Déu) and consists of 14 partners from 11 European countries.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>The projects mission is to maximize the use of biosamples, images and data for health research on the prevention, diagnosis and treatment of diseases. For this, these resources are available in a FAIR way: Findable, Accessible, Interoperable and Reusable. This is done in compliance with ethical, legal and privacy demands, and with active participation of donors, citizens and patients.</t>
+  </si>
+  <si>
+    <t>The objective of BioSHaRE-EU is to build upon tools and methods available to achieve solutions for researchers to use pooled data from different cohort and biobank studies. This, in order to obtain the very large sample sizes needed to investigate current questions in multifactorial diseases</t>
+  </si>
+  <si>
+    <t>The Canadian Partnership for Tomorrow’s Health (CanPath) is Canada’s largest
+population health cohort and a national platform for health research. Comprised of more
+than 330,000 volunteer participants, CanPath is a unique Canadian platform that allows
+scientists to explore how genetics, environment, lifestyle, and behaviour interact and
+contribute to the development of chronic disease and cancer. CanPath is hosted by the
+University of Toronto’s Dalla Lana School of Public Health with national funding from the
+Canadian Partnership Against Cancer.</t>
+  </si>
+  <si>
+    <t>The objective of COHORTS.SE is to coordinate all Swedish prospective population-based cohorts in a national infrastructure, thereby improving the reliability, quality and accessibility of valuable cohorts, for better-powered research with higher value to patients and populations.</t>
+  </si>
+  <si>
+    <t>The aim of CORDELIA is to generate a population database of more than 170,000 participants followed for more than 5 years, from Spanish cohorts with prospective follow-up.</t>
+  </si>
+  <si>
+    <t>The aim of EClipSE is to address the lack of statistical power within individual studies for specific analyses assessing relationships between data collected during life (e.g., health, cognitive, psychological, and genetic) and neuropathology at death.</t>
+  </si>
+  <si>
+    <t>EPHOR will develop methods and tools to characterise the working-life exposome. By applying these, better and more complete knowledge on the working-life exposome will be obtained. Through uniquely combining large-scale pooling of existing data (&gt;40 cohorts; ~ 21 million people) systematically looking at many types of exposure and diseases with the collection of new data in case studies in which the effects of working-life exposure on respiratory health in the general population and night shift workers will be investigated.</t>
+  </si>
+  <si>
+    <t>EPOSA is a collaborative study involving six cohort studies on ageing from six countries from North to South Europe. This initiative studies the personal and societal burden and its determinants of osteoarthritis in the aging European population using data from six population-based cohort studies across Europe.</t>
+  </si>
+  <si>
+    <t>The specific objectives of EUCAN-Connect are:
+* to deliver an open, federated data platform to deposit, curate and analyse cohort (meta)data that meets FAIR principles
+* to create a sustainable framework for long-term collaboration that enables better data-reuse and increased benefit to scientific communities worldwide</t>
+  </si>
+  <si>
+    <t>euCanSHare is a joint EU-Canada project to establish a cross-border data sharing and multi-cohort cardiovascular research platform. 
+Specifically, the project will integrate data infrastructures, IT solutions and data sources from EU, Canada and other countries into a web-based data access system with functionalities for increased efficiency in cardiovascular data-driven research. euCanSHare integrates more than 35 Canadian and European cohorts making up over 1 million records and actively seeks to expand to other regions. 
+euCanSHare key objectives are: data sharing, knowledge discovery, legal compliance, and community building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Gateway to Global Aging Data (g2aging.org) is a data and information platform developed to facilitate longitudinal and cross-country analyses on aging, especially those using the family of Health and Retirement Studies (HRS) around the world. To further this effort, the Gateway provides searchable metadata, extensive cross-survey documentation, downloadable harmonized microdata with variables standardized across surveys, and graphs and tables that enable users to instantly compare variables of interest over time, across countries, and against macro-level contextual information at no cost.
+</t>
+  </si>
+  <si>
+    <t>The aim of GenomEUtwin is to develop novel strategies to maximally utilize the unique features of twin cohorts, including the availability of longitudinal data and sample information about lifestyle and environmental factors, in the characterization of complex traits.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The HELIX project is funded to exploit novel tools and methods for characterisation of early-life exposure to a wide range of environmental hazards. These require integration and linkage with data on major child health outcomes, to develop an “Early-Life Exposome” approach.
+Six prospective birth cohort studies (INMA-Spain, RHEA-Greece, MoBa-Norway, EDEN-France, BiB-UK, KANC-Lithuania) are contributing to HELIX as the only realistic and feasible way to obtain the comprehensive, longitudinal, human data needed to build this early-life exposome. These cohorts have already collected large amounts of data as part of national and EU-funded projects. Results will be integrated with data from European cohorts (&gt;300,000 subjects) and registers, to estimate health impacts at the large European scale. This integration of the chemical, physical and molecular environment during critical early-life periods will lead to major improvements in health risk and impact assessments and thus to improved prevention strategies for vulnerable populations.
+</t>
+  </si>
+  <si>
+    <t>The specific objectives of the initiative are:
+- Conduct a set of harmonized, coordinated studies that will evaluate interventions along the life course from pre-conception to childhood to promote metabolic fitness and early development in children between 3-5 years of age;
+- Conduct mechanistic studies that will explain the effect of the selected interventions;
+- Conduct complementary policy and economic analyses;
+- Develop cross-country, cross-site collaborations that will provide a learning platform and training environment for young and talented scientists;
+- Use the generated evidence to guide policy and actions in the near future, and identify research and programmatic needs for long-term strategies.</t>
+  </si>
+  <si>
+    <t>The objectives of I3C are:
+1. Identify incident cardiovascular endpoints using self-reported morbidity validated by adjudication of medical records, and
+2. Identify decedents using the National Death Index and adjudicate cause of death for deceased participants.</t>
+  </si>
+  <si>
+    <t>The aim of I4C is to understand the aetiology and mechanistic underpinnings of childhood cancer by exploiting prospectively collected exposure and biomarker data.
+A summary is provided in the publication - 'The International Childhood Cancer Cohort Consortium (I4C): A research platform of prospective cohorts for studying the aetiology of childhood cancers' at the following link - https://onlinelibrary.wiley.com/doi/full/10.1111/ppe.12519</t>
+  </si>
+  <si>
+    <t>The aim of ICC-dementia is to harmonise centenarian and near-centenarian studies internationally to describe the cognitive and functional profiles of exceptionally old individuals, and ascertain the trajectories of decline and thereby the age-standardised prevalence and incidence of dementia.  The consortium is also interested in the genetic and environmental determinants of dementia-free exceptional longevity.</t>
+  </si>
+  <si>
+    <t>The aim of the IDEAR network is to investigate how determinants in later working life, during the retirement transition, and in early retirement influence for how long older individuals are able to live actively and healthily. 
+This will be done using by state of the art statistical modelling in well-established prospective occupational cohort studies, longitudinal ageing studies and registry data from Sweden, the UK, Finland, France and Denmark. 
+These studies represent countries in three different welfare regimes and cover up to several decades from mid-life, retirement, early old age, and the beginning of older-old age.</t>
+  </si>
+  <si>
+    <t>The maing objective of the IGEMS is to understand why early life adversity, and social factors such as isolation and loneliness, are associated with diverse outcomes including mortality, physical functioning (health, functional ability), and psychological functioning (well-being, cognition), particularly in later life.</t>
+  </si>
+  <si>
+    <t>To create a global network for translational research that utilizes large cohorts to enhance the understanding of the biological and genetic basis of disease and improve clinical care and population health. They also put in common challenges and better strategies in sharing data across cohorts.</t>
+  </si>
+  <si>
+    <t>The aim of interconnect is to develop a global data access and results sharing’ network that enables existing data to be readily used in cross-cohort analyses to understand population differences in the risk of diabetes and obesity.</t>
+  </si>
+  <si>
+    <t>The aim of InterLACE is to advance understandingof women’s reproductive health in relation to chronic disease risk by pooling individual participant data from several cohort and cross-sectional studies.</t>
+  </si>
+  <si>
+    <t>The overarching aim of the LIFEPATH project is to understand the determinants of diverging ageing pathways among individuals belonging to different socio-economic groups. This will be achieved via an original study design that integrates social science approaches with biology (including molecular epidemiology), using existing population cohorts and omics measurements (particularly epigenomics).</t>
+  </si>
+  <si>
+    <t>The objectives of MINDMAP are: 
+1. to harmonize and link data from population registries and cohort studies of mental health ageing in European cities to allow co-analysis of data, based on expertise by Erasmus MC with registry data and McGill University with survey data; 
+2. to develop a conceptual model of mental health in urban settings based on input from experts on mental health from multiple disciplinary perspectives and the integration of results from all work packages on the physical and social environmental, psychosocial, biological and genetic pathways linking the urban environment to mental health; and 
+3. to develop a methodological framework for the application of advanced causal inference and mediation analysis to study the causal impact of the urban environment on mental health.</t>
+  </si>
+  <si>
+    <t>The objective of NEAR is to improve the health, care, and well-being of older people by optimizing a national integration of the major Swedish longitudinal, population-based projects on the health and care of older people.</t>
+  </si>
+  <si>
+    <t>The overarching concept of OMEGA-NET is to create a network to optimize and integrate occupational, industrial, and population cohorts at the European level, and to provide a foundation for an enhanced evidence base for the identification of health risks and gains related to occupation and employment to foster safe and healthy preventive strategies and policies.
+Research Coordination Objectives and health
+Coordinate and integrate cohorts on occupational health in Europe:
+* Implement an online interactive tool with detailed information on existing cohorts
+* Facilitate work on harmonization of occupational exposure and standardization of health outcome information and new protocols for data collection
+* Promote stakeholder engagement from the start of the project.
+Capacity Building Objectives:
+* Connect scientific communities on occupational health in Europe
+* Provide networking and leadership opportunities for early career researchers, as well as researchers from COST Inclusiveness Target Countries
+* Provide training in occupational epidemiology and exposure assessment</t>
+  </si>
+  <si>
+    <t>The aim of ReACH is to provide resources in the form of a comprehensive web-based catalogue and an harmonization platform to optimize and expand the use of Canadian pregnancy and birth cohorts data and biological samples.</t>
+  </si>
+  <si>
+    <t>The objective of SAPRIN is to draw together and harmonise a network of South Africa’s health and demographic surveillance sites (HDSS) situated in rural and urban setting, each with a population of at least 100 000 individuals under surveillance.</t>
+  </si>
+  <si>
+    <t>The Social Inequality in Cancer (SIC) cohort study was established to determine path- ways through which socioeconomic position affects morbidity and mortality, in particular common subtypes of cancer.</t>
+  </si>
+  <si>
+    <t>To establish a genome epidemiological study platform for the research community with a health database and biobank, to investigate the genetic and environmental aetiology of common complex diseases in Koreans and causes of death with long-term follow-up. The ultimate goal of the KoGES was to develop comprehensive and applicable health care guidelines for common complex diseases in Koreans, reduce the burden of chronic diseases and improve the quality of life.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To enable the conduct of studies of medication use and outcomes in pregnancy.    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To maximise the use, value and impact of longitudinal studies to help improve our understanding of key social and biomedical challenges. </t>
+  </si>
+  <si>
+    <t>• harmonize pregnancy and birth cohort data for the 3D, MIREC and SBC studies • establish a collaborative research network on the topic of intra-uterine determinants of child health and development and on perinatal health services in Quebec and Shanghai (China) • establish an infrastructure of knowledge transfer and application between the partners and users of the network leading to updated guidelines, health policies, and knowledge transfer activities in clinical practice • reinforce the strategic positioning of academic and industrial partners in Quebec, China and internationally for providing access to new markets and expertise.</t>
+  </si>
+  <si>
+    <t>To understand the relationship between genetics, environmental exposures, and the etiology of disease through the establishment of a cohort, or population laboratory.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHANCES aims at combining and integrating ongoing cohort studies in order to produce evidence on ageing-related health characteristics and determinants in Europe and their socio-economic implications.   </t>
+  </si>
+  <si>
+    <t>The scientific goal of ECHO, a research program launched by the National Institutes of Health, is to understand the effects of a broad range of early environmental influences on child health and development. ECHO uses information from existing longitudinal research projects (cohorts), which will include more than 50,000 children from diverse backgrounds across the United States. Together, these cohorts follow participants from before they are born through childhood and adolescence. ECHO also supports a 17-state clinical trials network to test prevention and treatment strategies among children from rural and medically underserved backgrounds. Program Objectives + Improve the health of children and adolescents by conducting observational and interventional research that will inform high-impact programs, policies, and practices. + Institute best practices for conducting Team Science in the 21st century, giving researchers the tools to work collaboratively to improve child health.</t>
+  </si>
+  <si>
+    <t>Project aims to improve human health through genetic research, and ultimately identify new therapeutic targets and diagnostics for treating numerous diseases. The collaborative nature of the project is exceptional compare to many ongoing studies, and all the partners are working closely together to ensure appropriate transparency, data security and ownership.</t>
+  </si>
+  <si>
+    <t>GenomeAsia 100K plans to create reference genomes for Asian population as well as identify rare and frequent alleles associated with these populations. In the process, we hope to understand biology of disease and enable new therapeutic options which will have global impact. The first stage aims to sequence 10,000 Asian individuals for ethnic stratification. This will be followed by sequencing an additional 90,000 individuals and combined with clinical and phenotype information to allow deeper analysis of diseased and healthy individuals. Our founding partners have direct access to cohorts of samples with specific disease characteristics which will be especially useful during this second stage and even allow for studies across longer time periods.</t>
+  </si>
+  <si>
+    <t>1 Develop, evaluate and refine methodologies for assessing the effects of social, economic and health policies on the pattern and magnitude of health inequalities among socioeconomic groups. 2 Assess the differential health effects by socioeconomic group of natural policy experiments’ in the fields of unemployment and poverty reduction; tobacco and alcohol control; and access to education and preventive health care. 3 Synthesise the evidence from the findings of objectives 1-2, and actively engage users in the research in order to promote the transfer of knowledge for policy and practice with maximum effectiveness.</t>
+  </si>
+  <si>
+    <t>Tohoku Medical Megabank Organization was founded to establish an advanced medical system to foster the reconstruction from the Great East Japan Earthquake. The organization has been developing a biobank that combines medical and genome information during the process of rebuilding the community medical system and supporting health and welfare in the Tohoku area.</t>
+  </si>
+  <si>
+    <t>The outcome of the harmonization work leading to SAGE+ Wave 1 and SAGE+ Wave 2 is two common datasets that will allow a wide range of cross-country comparisons and evaluation of the predictors of transitions in various domains, from subjective health status and risk factors shifts, to evaluation in relationships between wealth and health in countries at different levels of development. The aim of this article is to present the analogous results for SAGE+ Wave 2 which extends and adds unique data to SAGE+ Wave 1. The harmonization process for SAGE+ Wave 2 builds on SAGE+ Wave 1 processes and follows the same methodology. SAGE+ Wave 2 included the two additional studies, CHARLS and LASI, whose variables were subjected to the same harmonization process as used in SAGE+ Wave 1 without encountering major deviations. The inclusion of these studies allowed the creation of some additional harmonized variables, such as verbal fluency, depression, emotional/psychiatric problems, cataracts, and hip fracture, for some studies.</t>
+  </si>
+  <si>
+    <t>The overall aim of the RECAP preterm Project is to improve the health, development and quality of life of children and adults born very preterm (VPT) or with a very low birth weight (VLBW). This aim will be achieved by combining extensive data from European cohort studies and around the world, which makes it possible to evaluate changes in outcomes over time while providing important information on how the evolution in care and survival of these high risk babies has changed their developmental outcomes and quality of life. We want to develop a better understanding of the origins of VPT/VLBW health and developmental outcomes as well as more effective, evidence-based, personalized interventions and prevention.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To identify effective pathways to compressing morbidity and optimising ageing.                                                                                                                         Four key foci, including dementia and cognition, mental health, sensory impairment, and mobility/activity limitations. </t>
+  </si>
+  <si>
+    <t>Consortium (HAVIC), and cited the following objectives: 1) prospective design, 2) common exposure metrics across cohorts, 3) common health assessment instruments across cohorts, and 4) methods for multisite integration.</t>
+  </si>
+  <si>
+    <t>The primary aim is to conduct high-quality analyses that produce, in an efficient and timely manner, reliable and valid findings across multiple cardiovascular and aging-related phenotypes.</t>
+  </si>
+  <si>
+    <t>The LIFESPAN project adopts a life-course perspective to examine the early life influences (birth order, parental age, family/sibling size, birth weight, birth length) on suicide, suicidal ideation, and suicide attempts in the general population. It comprises 3 complementary objectives: (1) to summarise available studies about the longitudinal relations between early-life influences and suicide mortality by applying meta-analysis, the statistical approach most informative for policymakers, allowing to go beyond the heterogeneity of existing studies; (2) to investigate the associations between early-life influences and suicidal ideation and attempts in adolescence and young adulthood with data from 3 longitudinal population-based cohorts (from Canada and France; up to 25 years follow-up); (3) to identify specific mediating pathways (targetable with new preventive interventions) linking early-life factors and suicide risk, using advances longitudinal mediation analysis techniques relying on growth curve modelling.</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>All cohort study health outcomes in relation to environmental and occupational exposures in agricultural settings with the exception of three general population cohorts involving a large number of agricultural populations or oversampling individuals in agricultural areas.</t>
+  </si>
+  <si>
+    <t>Each study includes one or more populations and provides data on health determinants and age-related events.</t>
+  </si>
+  <si>
+    <t>Cohorts with Genetic, epigenetic, transcriptome and metabolome data available.</t>
+  </si>
+  <si>
+    <t>Large biobanks or study cohorts with no specific health context.</t>
+  </si>
+  <si>
+    <t>Canadian regional cohorts that investigate environmental, lifestyle and genetic factors related to the development and progression of cancer and chronic diseases.</t>
+  </si>
+  <si>
+    <t>Swedish prospective population-based cohorts.</t>
+  </si>
+  <si>
+    <t>Spanish population-based cohort studies with information on common chronic disease risk factors and follow up for chronic diseases events.</t>
+  </si>
+  <si>
+    <t>European population-based longitudinal cohorts of older adults with a brain-donation program at death</t>
+  </si>
+  <si>
+    <t>Cohort studies with occupational history information.</t>
+  </si>
+  <si>
+    <t>Criteria for selection were a good representation of countries across Europe, different physical and social environments and health care systems. In addition, initially (for the post-harmonisation) a requirement was the existence of a running cohort study on older people</t>
+  </si>
+  <si>
+    <t>European cohorts of babies born very preterm or with very low birth weight (VPT/ VLBW cohorts)</t>
+  </si>
+  <si>
+    <t>The project brings together 35 cardiovascular cohorts from EU, Canada* and beyond, including sociodemographic data, biosamples, omics data (DNA/RNA/proteins), cardiac imaging, lifestyle, environmental data, physical measurements and clinical outcomes.</t>
+  </si>
+  <si>
+    <t>Cohort studies about aging and health, most of them harmonized ex-ante with the family of international Health and Retirement studies.</t>
+  </si>
+  <si>
+    <t>Twin cohorts with genomic, lifestyle and environmental information.</t>
+  </si>
+  <si>
+    <t>The project focus on studies based in the UK with life course data and specific ageing outcomes measured in midlife or old age and/or repeat measures of capability in later life</t>
+  </si>
+  <si>
+    <t>The selected cohorts were  included in the
+HELIX project because: (a) they could provide substantial
+existing longitudinal data from early pregnancy
+through childhood, (b) they could follow-up children
+at similar ages, (c) they could integrate questionnaires, biosampling and clinical examinations using common
+HELIX protocols and (d) they offered heterogeneity in
+terms of exposure and population characteristics.</t>
+  </si>
+  <si>
+    <t>Intervention cohorts established in Canada, China, India and South Africa that examine the effects of interventions starting preconception, during pregnancy and into early childhood on body composition of children at 5 years of age and measures of early child development.</t>
+  </si>
+  <si>
+    <t>long-term observational studies of risk factors for heart disease started in groups of school children.</t>
+  </si>
+  <si>
+    <t>Cohorts eligible for inclusion in the I4C need to recruit mothers during pregnancy or around delivery. Eligible cohorts must systematically ascertain cases of CC in the offspring and should include questionnaire and/or other exposure data that address key CC aetiology-related hypotheses. The specific goals and original outcomes of the individual cohorts (eg, pregnancy complications and/ or serious chronic childhood conditions) may vary, but critical data items include parental and offspring demographic, life style, medical, reproductive, environmental factors and parental occupational information. Specific responsibilities of newly joining or participating I4C cohorts include sharing of data (and biospecimens-if available) for current and future proposals.</t>
+  </si>
+  <si>
+    <t>Studies are eligible to participate in ICC-Dementia if they meet the following criteria:
+1.	The main focus is on individuals aged ≥95 years
+2.	Have a minimum sample of 80 individuals
+3.	Assessment includes measures of cognitive function and activities of daily living
+4.	Informed consent forms allow for de-identified data sharing with academic partners.
+All participating studies have the opportunity to participate in the analyses and to propose specific projects and papers.</t>
+  </si>
+  <si>
+    <t>Prospective occupational cohort studies</t>
+  </si>
+  <si>
+    <t>Cohorts involving twins with measures of physical health, cognitive health and emotional health, and measures of multiple facets of adult socioeconomic status (SES; e.g.occupation, education, financial strain)</t>
+  </si>
+  <si>
+    <t>Cohorts that recruit 100k participants or more, are disease-agnostic, have available biospecimens, and have longitudinal follow-up activities. Cohorts from under-represented populations and low and middle-income countries (LMICs) may not fit some of these criteria, so exceptions are made to be inclusive as possible.</t>
+  </si>
+  <si>
+    <t>Cohort studies with information of diabetes and obesity.</t>
+  </si>
+  <si>
+    <t>Observational studies, which had collected prospective or retrospective survey data on women’s reproductive health across the lifespan (such as ages at menarche, first birth, and natural menopause), sociodemographic and lifestyle factors, and chronic disease events, could contribute data to the InterLACE consortium, regardless of the sample size and ethnic background of participants.</t>
+  </si>
+  <si>
+    <t>LIFEPATH  includes information and biological samples from 17 cohorts, including several with extensive phenotyping and repeat biological
+samples, and a very large cohort  (1 million individuals) without biological samples  (WHIP,  from Italy). They were chosen for the combination of good measures of
+socioeconomic status,  risk factors for non-communicable diseases (NCDs) and biomarkers already measured  (or availability of blood samples for further testing).</t>
+  </si>
+  <si>
+    <t>Cohort studies with information on the urban environment and the individual determinants of mental wellbeing in older age.</t>
+  </si>
+  <si>
+    <t>Cohorts of health and care with at least seven years of follow-up time of older people in the Swedish population.</t>
+  </si>
+  <si>
+    <t>European occupational, industrial, and population, and registry-based cohorts with data on occupational exposures.</t>
+  </si>
+  <si>
+    <t>(1) recruit Canadian mothers and/or children; 
+(2) have a longitudinal design (i.e. at least one follow-up of participants after the initial collection event); 
+(3) have collected data (baseline or follow-up) after 2000; 
+(4) collect information on pregnancy and birth outcomes</t>
+  </si>
+  <si>
+    <t>Standardised, population-based data in geographically-defined sections of impoverished communities.</t>
+  </si>
+  <si>
+    <t>The inclusion criteria for enrolment in the SIC cohort were: a population-based study from Denmark with data on behavioural and biological risk factors for sub-types of cancer and other common outcomes (i.e. cardiovascular diseases); and a baseline examination after 1980, since socioeconomic information drawn from the central registries was only available after January 1980.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Community-dwellers and participants recruited from the national health examinee registry, men and women, aged ≥ 40 years at baseline. </t>
+  </si>
+  <si>
+    <t>Information on maternal and infant characteristics and medical care from the automated databases of the 11 health plans associated with the three FDA contract sites and birth certificate data obtained from the state departments of public health.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">People born in different regions of the UK throughout the 20th and 21st centuries. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pregnancy and birth population.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Healthy people around the world aged 40 years or more. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Most cohorts included in the consortium included subjects aged 50 or over, and separate analyses were conducted, if deemed necessary, on health-related characteristics and determinants in subjects aged 50-59, 60-69, and 70+ years.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More than 50,000 children from diverse racial, geographic and socioeconomic backgrounds.    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biological samples of finnish population </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genomic information for Asian populations  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">150,000 healthy Japanese participants with informed consent in Miyagi and Iwate prefectures. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">50+ general population. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Children and adults born very preterm (VPT) or with a very low birth weight (VLBW).  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australian adults 45+ years old. </t>
+  </si>
+  <si>
+    <t>Australia, Canada, Chile, Costa Rica, Denmark, France, New Zealand, Norway, South Korea, South Africa, United Kingdom, United States</t>
+  </si>
+  <si>
+    <t>Cuba, Mexico, Dominican Republic, Puerto Rico, China, Peru, India, Venezuela, Austria, Australia, Greece, Spain, Finland, Poland, United Kingdom, Russia, Lithuania, Czechia, United States, Japan, Ghana, Netherlands, South Korea, South Africa, Denmark, Hungary, Sweden, Switzerland, Ireland, Estonia, Belgium, Israel, Slovenia, Croatia, Luxembourg, Portugal, France, Germany, Italy</t>
+  </si>
+  <si>
+    <t>United Kingdom, Finland</t>
+  </si>
+  <si>
+    <t>Netherlands, Spain, United Kingdom, Denmark, Sweden, Belgium, Norway, France, Finland, Greece, Germany, Cyprus</t>
+  </si>
+  <si>
+    <t>Germany, Italy, Netherlands, Spain, United Kingdom, Sweden</t>
+  </si>
+  <si>
+    <t>Canada, Norway, France, Denmark, Estonia, Germany, Greece, Italy, Lithuania, Poland, Russia, Ireland, Portugal, Belgium, Spain, Sweden, Netherlands, United Kingdom, Finland, Australia</t>
+  </si>
+  <si>
+    <t>Germany, United Kingdom, Finland, Estonia, Denmark, Italy, Spain, Lithuania, Australia, Sweden, Russia, Poland, France, Norway, Canada</t>
+  </si>
+  <si>
+    <t>United States, Mexico, Israel, Costa Rica, South Korea, Japan, China, India, United Kingdom, Austria, Belgium, Croatia, Cyprus, Czechia, Denmark, Estonia, Finland, France, Germany, Greece, Hungary, Italy, Latvia, Lithuania, Luxembourg, Malta, Netherlands, Poland, Portugal, Romania, Slovakia, Slovenia, Spain, Sweden, Switzerland, Ireland, Indonesia, Ghana, Russia, South Africa, Brazil, Thailand, Malaysia</t>
+  </si>
+  <si>
+    <t>Denmark, Finland, Italy, Netherlands, Norway, United Kingdom, Australia, Sweden</t>
+  </si>
+  <si>
+    <t>France, Greece, Lithuania, Norway, Spain, United Kingdom</t>
+  </si>
+  <si>
+    <t>United States, Finland, Australia</t>
+  </si>
+  <si>
+    <t>Australia, Denmark, Brazil, China, France, Italy, Israel, Japan, Norway, United Kingdom, United States</t>
+  </si>
+  <si>
+    <t>Sweden, United Kingdom, Finland, France, Denmark</t>
+  </si>
+  <si>
+    <t>Sweden, Denmark, Finland, United States, Australia</t>
+  </si>
+  <si>
+    <t>Australia, United Kingdom, Denmark, France, Japan, United States, Lebanon, Spain, Sweden, Morocco, China</t>
+  </si>
+  <si>
+    <t>United Kingdom, Ireland, Portugal, France, Switzerland, Italy, Finland, United States, Australia</t>
+  </si>
+  <si>
+    <t>Canada, Netherlands, Russia, Poland, Norway, Germany, United States, France, Italy</t>
+  </si>
+  <si>
+    <t>Argentina, Australia, Belgium, Brazil, Canada, Chile, Croatia, Egypt, Estonia, Germany, Greece, Hungary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Korea, Vietnam, Cambodia, Japan, China </t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States of America    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Kingdom </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canada, China   </t>
+  </si>
+  <si>
+    <t>Bangladesh, Japan, Taiwan, South Korea, China, India, Singapore, Iran, Mongolia, Singapore Malaysia,, the United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Kingdom, The Netherlands, Germany, France, Denmark, Greece, Finland, Norway, Sweden, United States   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finland </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asia  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tohoku (region of Japan) </t>
+  </si>
+  <si>
+    <t>China, Ghana, India, Mexico, the Russian Federation, South Africa, England, USA, Austria, Belgium, Denmark, France, Germany, Greece, Italy, Switzerland, The Netherlands, Spain, Sweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">US, Sweden, Finland      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canada, France        </t>
+  </si>
+  <si>
+    <t>0 - 150</t>
+  </si>
+  <si>
+    <t>18 - 120</t>
+  </si>
+  <si>
+    <t>0 - 120</t>
+  </si>
+  <si>
+    <t>30 - 74</t>
+  </si>
+  <si>
+    <t>0 - 90</t>
+  </si>
+  <si>
+    <t>35 - 84</t>
+  </si>
+  <si>
+    <t>65 - 150</t>
+  </si>
+  <si>
+    <t>65 - 85</t>
+  </si>
+  <si>
+    <t>45+</t>
+  </si>
+  <si>
+    <t>20 - 85</t>
+  </si>
+  <si>
+    <t>50 - 90</t>
+  </si>
+  <si>
+    <t>0 - 12</t>
+  </si>
+  <si>
+    <t>3 - 19</t>
+  </si>
+  <si>
+    <t>0 - 30</t>
+  </si>
+  <si>
+    <t>95+</t>
+  </si>
+  <si>
+    <t>10 - 74</t>
+  </si>
+  <si>
+    <t>14 - 103</t>
+  </si>
+  <si>
+    <t>30 - 75</t>
+  </si>
+  <si>
+    <t>26+</t>
+  </si>
+  <si>
+    <t>0 - 45</t>
+  </si>
+  <si>
+    <t>20 - 93</t>
+  </si>
+  <si>
+    <t>40+</t>
+  </si>
+  <si>
+    <t>0 - 17</t>
+  </si>
+  <si>
+    <t>45 - 106</t>
+  </si>
+  <si>
+    <t>32+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -6428,4 +7437,2725 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D1" t="s">
+        <v>444</v>
+      </c>
+      <c r="E1" t="s">
+        <v>445</v>
+      </c>
+      <c r="F1" t="s">
+        <v>446</v>
+      </c>
+      <c r="G1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H1" t="s">
+        <v>448</v>
+      </c>
+      <c r="I1" t="s">
+        <v>449</v>
+      </c>
+      <c r="J1" t="s">
+        <v>450</v>
+      </c>
+      <c r="K1" t="s">
+        <v>451</v>
+      </c>
+      <c r="L1" t="s">
+        <v>452</v>
+      </c>
+      <c r="M1" t="s">
+        <v>453</v>
+      </c>
+      <c r="N1" t="s">
+        <v>454</v>
+      </c>
+      <c r="O1" t="s">
+        <v>455</v>
+      </c>
+      <c r="P1" t="s">
+        <v>456</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>457</v>
+      </c>
+      <c r="R1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>459</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2" t="s">
+        <v>608</v>
+      </c>
+      <c r="G2" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>656</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1300000.0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>316270.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>150.0</v>
+      </c>
+      <c r="N2"/>
+      <c r="O2" t="s">
+        <v>658</v>
+      </c>
+      <c r="P2" t="s">
+        <v>703</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>460</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>559</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3" t="s">
+        <v>609</v>
+      </c>
+      <c r="G3" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>656</v>
+      </c>
+      <c r="J3" t="n">
+        <v>411000.0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>411000.0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>120.0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>180.0</v>
+      </c>
+      <c r="O3" t="s">
+        <v>659</v>
+      </c>
+      <c r="P3" t="s">
+        <v>704</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="R3" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>461</v>
+      </c>
+      <c r="B4" t="s">
+        <v>517</v>
+      </c>
+      <c r="C4" t="s">
+        <v>517</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4"/>
+      <c r="F4" t="s">
+        <v>610</v>
+      </c>
+      <c r="G4" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>657</v>
+      </c>
+      <c r="J4" t="n">
+        <v>700.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>700.0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>120.0</v>
+      </c>
+      <c r="N4"/>
+      <c r="O4" t="s">
+        <v>660</v>
+      </c>
+      <c r="P4" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R4" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>462</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>560</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5" t="s">
+        <v>611</v>
+      </c>
+      <c r="G5" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>657</v>
+      </c>
+      <c r="J5" t="n">
+        <v>935227.0</v>
+      </c>
+      <c r="K5"/>
+      <c r="L5" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="M5"/>
+      <c r="N5" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>661</v>
+      </c>
+      <c r="P5" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="R5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>463</v>
+      </c>
+      <c r="B6" t="s">
+        <v>518</v>
+      </c>
+      <c r="C6" t="s">
+        <v>518</v>
+      </c>
+      <c r="D6" t="s">
+        <v>561</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6" t="s">
+        <v>612</v>
+      </c>
+      <c r="G6" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>656</v>
+      </c>
+      <c r="J6" t="n">
+        <v>386641.0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>328700.0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>74.0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>2840.0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>662</v>
+      </c>
+      <c r="P6" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R6" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>464</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>562</v>
+      </c>
+      <c r="E7"/>
+      <c r="F7" t="s">
+        <v>613</v>
+      </c>
+      <c r="G7" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>656</v>
+      </c>
+      <c r="J7" t="n">
+        <v>950000.0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>950000.0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="O7" t="s">
+        <v>663</v>
+      </c>
+      <c r="P7" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R7" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>465</v>
+      </c>
+      <c r="B8" t="s">
+        <v>519</v>
+      </c>
+      <c r="C8" t="s">
+        <v>519</v>
+      </c>
+      <c r="D8" t="s">
+        <v>563</v>
+      </c>
+      <c r="E8"/>
+      <c r="F8" t="s">
+        <v>614</v>
+      </c>
+      <c r="G8" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>656</v>
+      </c>
+      <c r="J8" t="n">
+        <v>188000.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>188000.0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>84.0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>664</v>
+      </c>
+      <c r="P8" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R8" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>466</v>
+      </c>
+      <c r="B9" t="s">
+        <v>520</v>
+      </c>
+      <c r="C9" t="s">
+        <v>520</v>
+      </c>
+      <c r="D9" t="s">
+        <v>564</v>
+      </c>
+      <c r="E9"/>
+      <c r="F9" t="s">
+        <v>615</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>657</v>
+      </c>
+      <c r="J9" t="n">
+        <v>987.0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>987.0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>150.0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="O9" t="s">
+        <v>665</v>
+      </c>
+      <c r="P9" t="s">
+        <v>705</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="R9" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>467</v>
+      </c>
+      <c r="B10" t="s">
+        <v>521</v>
+      </c>
+      <c r="C10" t="s">
+        <v>521</v>
+      </c>
+      <c r="D10" t="s">
+        <v>565</v>
+      </c>
+      <c r="E10"/>
+      <c r="F10" t="s">
+        <v>616</v>
+      </c>
+      <c r="G10" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>656</v>
+      </c>
+      <c r="J10" t="n">
+        <v>2.1E7</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O10" t="s">
+        <v>666</v>
+      </c>
+      <c r="P10" t="s">
+        <v>706</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="R10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>468</v>
+      </c>
+      <c r="B11" t="s">
+        <v>522</v>
+      </c>
+      <c r="C11" t="s">
+        <v>522</v>
+      </c>
+      <c r="D11" t="s">
+        <v>566</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11" t="s">
+        <v>617</v>
+      </c>
+      <c r="G11" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>657</v>
+      </c>
+      <c r="J11" t="n">
+        <v>2941.0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1949.0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>500.0</v>
+      </c>
+      <c r="O11" t="s">
+        <v>667</v>
+      </c>
+      <c r="P11" t="s">
+        <v>707</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="R11" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>469</v>
+      </c>
+      <c r="B12" t="s">
+        <v>523</v>
+      </c>
+      <c r="C12" t="s">
+        <v>523</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12"/>
+      <c r="F12" t="s">
+        <v>618</v>
+      </c>
+      <c r="G12" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>656</v>
+      </c>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O12" t="s">
+        <v>668</v>
+      </c>
+      <c r="P12" t="s">
+        <v>708</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="R12"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>470</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>598</v>
+      </c>
+      <c r="F13" t="s">
+        <v>619</v>
+      </c>
+      <c r="G13" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="H13"/>
+      <c r="I13" t="s">
+        <v>656</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1000000.0</v>
+      </c>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13" t="s">
+        <v>669</v>
+      </c>
+      <c r="P13" t="s">
+        <v>709</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="R13"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>471</v>
+      </c>
+      <c r="B14" t="s">
+        <v>524</v>
+      </c>
+      <c r="C14" t="s">
+        <v>524</v>
+      </c>
+      <c r="D14" t="s">
+        <v>567</v>
+      </c>
+      <c r="E14" t="s">
+        <v>599</v>
+      </c>
+      <c r="F14" t="s">
+        <v>620</v>
+      </c>
+      <c r="G14" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>656</v>
+      </c>
+      <c r="J14" t="n">
+        <v>351000.0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>351000.0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="M14"/>
+      <c r="N14" t="n">
+        <v>37000.0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>670</v>
+      </c>
+      <c r="P14" t="s">
+        <v>710</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="R14" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>472</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15"/>
+      <c r="F15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G15" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>657</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1190000.0</v>
+      </c>
+      <c r="K15"/>
+      <c r="L15" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="N15"/>
+      <c r="O15" t="s">
+        <v>671</v>
+      </c>
+      <c r="P15" t="s">
+        <v>711</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="R15" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>473</v>
+      </c>
+      <c r="B16" t="s">
+        <v>525</v>
+      </c>
+      <c r="C16" t="s">
+        <v>525</v>
+      </c>
+      <c r="D16" t="s">
+        <v>568</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>657</v>
+      </c>
+      <c r="J16" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="K16"/>
+      <c r="L16" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="N16"/>
+      <c r="O16" t="s">
+        <v>672</v>
+      </c>
+      <c r="P16" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R16" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>474</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>569</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>622</v>
+      </c>
+      <c r="G17" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>657</v>
+      </c>
+      <c r="J17" t="n">
+        <v>32000.0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>32000.0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="N17"/>
+      <c r="O17" t="s">
+        <v>673</v>
+      </c>
+      <c r="P17" t="s">
+        <v>712</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="R17" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>475</v>
+      </c>
+      <c r="B18" t="s">
+        <v>526</v>
+      </c>
+      <c r="C18" t="s">
+        <v>526</v>
+      </c>
+      <c r="D18" t="s">
+        <v>570</v>
+      </c>
+      <c r="E18"/>
+      <c r="F18" t="s">
+        <v>623</v>
+      </c>
+      <c r="G18" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>657</v>
+      </c>
+      <c r="J18" t="n">
+        <v>22730.0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>22000.0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="M18"/>
+      <c r="N18" t="n">
+        <v>1043.0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>674</v>
+      </c>
+      <c r="P18" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="R18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>476</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>571</v>
+      </c>
+      <c r="E19"/>
+      <c r="F19" t="s">
+        <v>624</v>
+      </c>
+      <c r="G19" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>657</v>
+      </c>
+      <c r="J19" t="n">
+        <v>42189.0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>31000.0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="N19" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>675</v>
+      </c>
+      <c r="P19" t="s">
+        <v>713</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="R19" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>477</v>
+      </c>
+      <c r="B20" t="s">
+        <v>527</v>
+      </c>
+      <c r="C20" t="s">
+        <v>527</v>
+      </c>
+      <c r="D20" t="s">
+        <v>572</v>
+      </c>
+      <c r="E20"/>
+      <c r="F20" t="s">
+        <v>625</v>
+      </c>
+      <c r="G20" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>656</v>
+      </c>
+      <c r="J20" t="n">
+        <v>388120.0</v>
+      </c>
+      <c r="K20"/>
+      <c r="L20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="N20" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="O20" t="s">
+        <v>676</v>
+      </c>
+      <c r="P20" t="s">
+        <v>714</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R20" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>478</v>
+      </c>
+      <c r="B21" t="s">
+        <v>528</v>
+      </c>
+      <c r="C21" t="s">
+        <v>528</v>
+      </c>
+      <c r="D21" t="s">
+        <v>573</v>
+      </c>
+      <c r="E21" t="s">
+        <v>600</v>
+      </c>
+      <c r="F21" t="s">
+        <v>626</v>
+      </c>
+      <c r="G21" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>656</v>
+      </c>
+      <c r="J21" t="n">
+        <v>7960.0</v>
+      </c>
+      <c r="K21"/>
+      <c r="L21" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21" t="s">
+        <v>677</v>
+      </c>
+      <c r="P21"/>
+      <c r="Q21" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R21" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>479</v>
+      </c>
+      <c r="B22" t="s">
+        <v>529</v>
+      </c>
+      <c r="C22" t="s">
+        <v>529</v>
+      </c>
+      <c r="D22" t="s">
+        <v>574</v>
+      </c>
+      <c r="E22"/>
+      <c r="F22" t="s">
+        <v>627</v>
+      </c>
+      <c r="G22" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>657</v>
+      </c>
+      <c r="J22" t="n">
+        <v>5000000.0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>150000.0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="M22" t="n">
+        <v>74.0</v>
+      </c>
+      <c r="N22" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="O22" t="s">
+        <v>678</v>
+      </c>
+      <c r="P22" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R22" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>480</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>575</v>
+      </c>
+      <c r="E23"/>
+      <c r="F23" t="s">
+        <v>628</v>
+      </c>
+      <c r="G23" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>656</v>
+      </c>
+      <c r="J23" t="n">
+        <v>76233.0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>76233.0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="N23" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="O23" t="s">
+        <v>679</v>
+      </c>
+      <c r="P23" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R23" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>481</v>
+      </c>
+      <c r="B24" t="s">
+        <v>530</v>
+      </c>
+      <c r="C24" t="s">
+        <v>530</v>
+      </c>
+      <c r="D24" t="s">
+        <v>576</v>
+      </c>
+      <c r="E24"/>
+      <c r="F24" t="s">
+        <v>629</v>
+      </c>
+      <c r="G24" t="n">
+        <v>67.0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>656</v>
+      </c>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>150.0</v>
+      </c>
+      <c r="N24"/>
+      <c r="O24" t="s">
+        <v>680</v>
+      </c>
+      <c r="P24"/>
+      <c r="Q24" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R24" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>482</v>
+      </c>
+      <c r="B25" t="s">
+        <v>531</v>
+      </c>
+      <c r="C25" t="s">
+        <v>531</v>
+      </c>
+      <c r="D25" t="s">
+        <v>531</v>
+      </c>
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" t="s">
+        <v>630</v>
+      </c>
+      <c r="G25" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>657</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1000000.0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1000000.0</v>
+      </c>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="O25" t="s">
+        <v>681</v>
+      </c>
+      <c r="P25"/>
+      <c r="Q25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R25"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>483</v>
+      </c>
+      <c r="B26" t="s">
+        <v>532</v>
+      </c>
+      <c r="C26" t="s">
+        <v>532</v>
+      </c>
+      <c r="D26" t="s">
+        <v>577</v>
+      </c>
+      <c r="E26" t="s">
+        <v>601</v>
+      </c>
+      <c r="F26" t="s">
+        <v>631</v>
+      </c>
+      <c r="G26" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>656</v>
+      </c>
+      <c r="J26" t="n">
+        <v>839666.0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>839666.0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="M26" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="N26" t="n">
+        <v>1300.0</v>
+      </c>
+      <c r="O26" t="s">
+        <v>682</v>
+      </c>
+      <c r="P26" t="s">
+        <v>717</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R26" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>484</v>
+      </c>
+      <c r="B27" t="s">
+        <v>533</v>
+      </c>
+      <c r="C27" t="s">
+        <v>533</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27"/>
+      <c r="F27" t="s">
+        <v>632</v>
+      </c>
+      <c r="G27" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>657</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1941000.0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>102774.0</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M27" t="n">
+        <v>150.0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>270.0</v>
+      </c>
+      <c r="O27" t="s">
+        <v>683</v>
+      </c>
+      <c r="P27" t="s">
+        <v>718</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="R27" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>485</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" t="s">
+        <v>578</v>
+      </c>
+      <c r="E28"/>
+      <c r="F28" t="s">
+        <v>633</v>
+      </c>
+      <c r="G28" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>657</v>
+      </c>
+      <c r="J28" t="n">
+        <v>2662777.0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>2662777.0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="M28"/>
+      <c r="N28" t="n">
+        <v>2560.0</v>
+      </c>
+      <c r="O28" t="s">
+        <v>684</v>
+      </c>
+      <c r="P28" t="s">
+        <v>719</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="R28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>486</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" t="s">
+        <v>579</v>
+      </c>
+      <c r="E29"/>
+      <c r="F29" t="s">
+        <v>634</v>
+      </c>
+      <c r="G29" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>656</v>
+      </c>
+      <c r="J29" t="n">
+        <v>190268.0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L29" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29" t="s">
+        <v>685</v>
+      </c>
+      <c r="P29" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R29" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>487</v>
+      </c>
+      <c r="B30" t="s">
+        <v>534</v>
+      </c>
+      <c r="C30" t="s">
+        <v>534</v>
+      </c>
+      <c r="D30" t="s">
+        <v>580</v>
+      </c>
+      <c r="E30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" t="s">
+        <v>635</v>
+      </c>
+      <c r="G30"/>
+      <c r="H30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>656</v>
+      </c>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30" t="s">
+        <v>686</v>
+      </c>
+      <c r="P30"/>
+      <c r="Q30" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R30"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>488</v>
+      </c>
+      <c r="B31" t="s">
+        <v>535</v>
+      </c>
+      <c r="C31" t="s">
+        <v>535</v>
+      </c>
+      <c r="D31" t="s">
+        <v>581</v>
+      </c>
+      <c r="E31" t="s">
+        <v>602</v>
+      </c>
+      <c r="F31" t="s">
+        <v>636</v>
+      </c>
+      <c r="G31" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="I31" t="s">
+        <v>656</v>
+      </c>
+      <c r="J31" t="n">
+        <v>89889.0</v>
+      </c>
+      <c r="K31"/>
+      <c r="L31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M31" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="N31"/>
+      <c r="O31" t="s">
+        <v>687</v>
+      </c>
+      <c r="P31" t="s">
+        <v>720</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="R31" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>489</v>
+      </c>
+      <c r="B32" t="s">
+        <v>536</v>
+      </c>
+      <c r="C32" t="s">
+        <v>536</v>
+      </c>
+      <c r="D32" t="s">
+        <v>582</v>
+      </c>
+      <c r="E32"/>
+      <c r="F32" t="s">
+        <v>637</v>
+      </c>
+      <c r="G32" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I32" t="s">
+        <v>656</v>
+      </c>
+      <c r="J32" t="n">
+        <v>315000.0</v>
+      </c>
+      <c r="K32" t="n">
+        <v>315000.0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M32" t="n">
+        <v>120.0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="O32" t="s">
+        <v>688</v>
+      </c>
+      <c r="P32" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R32" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>490</v>
+      </c>
+      <c r="B33" t="s">
+        <v>537</v>
+      </c>
+      <c r="C33" t="s">
+        <v>537</v>
+      </c>
+      <c r="D33" t="s">
+        <v>583</v>
+      </c>
+      <c r="E33"/>
+      <c r="F33" t="s">
+        <v>638</v>
+      </c>
+      <c r="G33" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>657</v>
+      </c>
+      <c r="J33" t="n">
+        <v>83006.0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>83006.0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>93.0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="O33" t="s">
+        <v>689</v>
+      </c>
+      <c r="P33" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R33" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>491</v>
+      </c>
+      <c r="B34" t="s">
+        <v>538</v>
+      </c>
+      <c r="C34" t="s">
+        <v>538</v>
+      </c>
+      <c r="D34" t="s">
+        <v>584</v>
+      </c>
+      <c r="E34"/>
+      <c r="F34" t="s">
+        <v>639</v>
+      </c>
+      <c r="G34" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H34"/>
+      <c r="I34" t="s">
+        <v>657</v>
+      </c>
+      <c r="J34" t="n">
+        <v>245000.0</v>
+      </c>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34" t="s">
+        <v>690</v>
+      </c>
+      <c r="P34" t="s">
+        <v>721</v>
+      </c>
+      <c r="Q34"/>
+      <c r="R34"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>492</v>
+      </c>
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" t="s">
+        <v>585</v>
+      </c>
+      <c r="E35"/>
+      <c r="F35" t="s">
+        <v>640</v>
+      </c>
+      <c r="G35" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35" t="n">
+        <v>1221156.0</v>
+      </c>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35" t="s">
+        <v>691</v>
+      </c>
+      <c r="P35" t="s">
+        <v>722</v>
+      </c>
+      <c r="Q35"/>
+      <c r="R35"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>493</v>
+      </c>
+      <c r="B36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" t="s">
+        <v>586</v>
+      </c>
+      <c r="E36"/>
+      <c r="F36" t="s">
+        <v>641</v>
+      </c>
+      <c r="G36" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36" t="n">
+        <v>119952.0</v>
+      </c>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="O36" t="s">
+        <v>692</v>
+      </c>
+      <c r="P36" t="s">
+        <v>723</v>
+      </c>
+      <c r="Q36"/>
+      <c r="R36"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>494</v>
+      </c>
+      <c r="B37" t="s">
+        <v>539</v>
+      </c>
+      <c r="C37" t="s">
+        <v>539</v>
+      </c>
+      <c r="D37" t="s">
+        <v>106</v>
+      </c>
+      <c r="E37" t="s">
+        <v>603</v>
+      </c>
+      <c r="F37" t="s">
+        <v>108</v>
+      </c>
+      <c r="G37" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I37" t="s">
+        <v>656</v>
+      </c>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>495</v>
+      </c>
+      <c r="B38" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" t="s">
+        <v>587</v>
+      </c>
+      <c r="E38"/>
+      <c r="F38" t="s">
+        <v>642</v>
+      </c>
+      <c r="G38" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38" t="n">
+        <v>16527.0</v>
+      </c>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38" t="s">
+        <v>693</v>
+      </c>
+      <c r="P38" t="s">
+        <v>724</v>
+      </c>
+      <c r="Q38"/>
+      <c r="R38"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>496</v>
+      </c>
+      <c r="B39" t="s">
+        <v>540</v>
+      </c>
+      <c r="C39"/>
+      <c r="D39" t="s">
+        <v>540</v>
+      </c>
+      <c r="E39"/>
+      <c r="F39" t="s">
+        <v>643</v>
+      </c>
+      <c r="G39" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>656</v>
+      </c>
+      <c r="J39" t="n">
+        <v>1221985.0</v>
+      </c>
+      <c r="K39" t="n">
+        <v>1221985.0</v>
+      </c>
+      <c r="L39" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="M39"/>
+      <c r="N39" t="n">
+        <v>600.0</v>
+      </c>
+      <c r="O39" t="s">
+        <v>694</v>
+      </c>
+      <c r="P39" t="s">
+        <v>725</v>
+      </c>
+      <c r="Q39"/>
+      <c r="R39" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>497</v>
+      </c>
+      <c r="B40" t="s">
+        <v>541</v>
+      </c>
+      <c r="C40" t="s">
+        <v>541</v>
+      </c>
+      <c r="D40" t="s">
+        <v>588</v>
+      </c>
+      <c r="E40"/>
+      <c r="F40" t="s">
+        <v>644</v>
+      </c>
+      <c r="G40" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="I40" t="s">
+        <v>657</v>
+      </c>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="M40"/>
+      <c r="N40" t="n">
+        <v>323.0</v>
+      </c>
+      <c r="O40" t="s">
+        <v>695</v>
+      </c>
+      <c r="P40" t="s">
+        <v>726</v>
+      </c>
+      <c r="Q40"/>
+      <c r="R40" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>498</v>
+      </c>
+      <c r="B41" t="s">
+        <v>542</v>
+      </c>
+      <c r="C41" t="s">
+        <v>542</v>
+      </c>
+      <c r="D41" t="s">
+        <v>589</v>
+      </c>
+      <c r="E41"/>
+      <c r="F41" t="s">
+        <v>645</v>
+      </c>
+      <c r="G41" t="n">
+        <v>84.0</v>
+      </c>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41" t="n">
+        <v>50000.0</v>
+      </c>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41" t="s">
+        <v>696</v>
+      </c>
+      <c r="P41" t="s">
+        <v>727</v>
+      </c>
+      <c r="Q41"/>
+      <c r="R41"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>499</v>
+      </c>
+      <c r="B42" t="s">
+        <v>543</v>
+      </c>
+      <c r="C42" t="s">
+        <v>543</v>
+      </c>
+      <c r="D42" t="s">
+        <v>590</v>
+      </c>
+      <c r="E42"/>
+      <c r="F42" t="s">
+        <v>646</v>
+      </c>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42" t="s">
+        <v>697</v>
+      </c>
+      <c r="P42" t="s">
+        <v>728</v>
+      </c>
+      <c r="Q42"/>
+      <c r="R42"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>500</v>
+      </c>
+      <c r="B43" t="s">
+        <v>544</v>
+      </c>
+      <c r="C43"/>
+      <c r="D43" t="s">
+        <v>544</v>
+      </c>
+      <c r="E43"/>
+      <c r="F43" t="s">
+        <v>647</v>
+      </c>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43" t="s">
+        <v>698</v>
+      </c>
+      <c r="P43" t="s">
+        <v>729</v>
+      </c>
+      <c r="Q43"/>
+      <c r="R43"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>501</v>
+      </c>
+      <c r="B44" t="s">
+        <v>545</v>
+      </c>
+      <c r="C44" t="s">
+        <v>545</v>
+      </c>
+      <c r="D44" t="s">
+        <v>591</v>
+      </c>
+      <c r="E44" t="s">
+        <v>604</v>
+      </c>
+      <c r="F44" t="s">
+        <v>648</v>
+      </c>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44" t="s">
+        <v>657</v>
+      </c>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
+      <c r="P44"/>
+      <c r="Q44"/>
+      <c r="R44"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>502</v>
+      </c>
+      <c r="B45" t="s">
+        <v>546</v>
+      </c>
+      <c r="C45"/>
+      <c r="D45" t="s">
+        <v>546</v>
+      </c>
+      <c r="E45"/>
+      <c r="F45" t="s">
+        <v>649</v>
+      </c>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45" t="s">
+        <v>657</v>
+      </c>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45" t="s">
+        <v>699</v>
+      </c>
+      <c r="P45" t="s">
+        <v>730</v>
+      </c>
+      <c r="Q45"/>
+      <c r="R45"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>503</v>
+      </c>
+      <c r="B46" t="s">
+        <v>252</v>
+      </c>
+      <c r="C46"/>
+      <c r="D46" t="s">
+        <v>252</v>
+      </c>
+      <c r="E46" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" t="s">
+        <v>253</v>
+      </c>
+      <c r="G46"/>
+      <c r="H46" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="I46" t="s">
+        <v>656</v>
+      </c>
+      <c r="J46" t="n">
+        <v>250000.0</v>
+      </c>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+      <c r="O46" t="s">
+        <v>258</v>
+      </c>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>504</v>
+      </c>
+      <c r="B47" t="s">
+        <v>547</v>
+      </c>
+      <c r="C47" t="s">
+        <v>547</v>
+      </c>
+      <c r="D47" t="s">
+        <v>592</v>
+      </c>
+      <c r="E47"/>
+      <c r="F47" t="s">
+        <v>650</v>
+      </c>
+      <c r="G47" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>657</v>
+      </c>
+      <c r="J47" t="n">
+        <v>136128.0</v>
+      </c>
+      <c r="K47" t="n">
+        <v>136128.0</v>
+      </c>
+      <c r="L47" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="M47"/>
+      <c r="N47"/>
+      <c r="O47" t="s">
+        <v>700</v>
+      </c>
+      <c r="P47" t="s">
+        <v>731</v>
+      </c>
+      <c r="Q47"/>
+      <c r="R47" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>505</v>
+      </c>
+      <c r="B48" t="s">
+        <v>548</v>
+      </c>
+      <c r="C48" t="s">
+        <v>548</v>
+      </c>
+      <c r="D48" t="s">
+        <v>593</v>
+      </c>
+      <c r="E48" t="s">
+        <v>605</v>
+      </c>
+      <c r="F48" t="s">
+        <v>651</v>
+      </c>
+      <c r="G48" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
+      <c r="O48" t="s">
+        <v>701</v>
+      </c>
+      <c r="P48"/>
+      <c r="Q48"/>
+      <c r="R48"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>506</v>
+      </c>
+      <c r="B49" t="s">
+        <v>280</v>
+      </c>
+      <c r="C49" t="s">
+        <v>280</v>
+      </c>
+      <c r="D49" t="s">
+        <v>280</v>
+      </c>
+      <c r="E49" t="s">
+        <v>606</v>
+      </c>
+      <c r="F49" t="s">
+        <v>282</v>
+      </c>
+      <c r="G49" t="n">
+        <v>69.0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>69.0</v>
+      </c>
+      <c r="I49" t="s">
+        <v>656</v>
+      </c>
+      <c r="J49" t="n">
+        <v>320000.0</v>
+      </c>
+      <c r="K49" t="n">
+        <v>320000.0</v>
+      </c>
+      <c r="L49" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="M49"/>
+      <c r="N49" t="n">
+        <v>281.0</v>
+      </c>
+      <c r="O49" t="s">
+        <v>283</v>
+      </c>
+      <c r="P49"/>
+      <c r="Q49"/>
+      <c r="R49" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>507</v>
+      </c>
+      <c r="B50" t="s">
+        <v>549</v>
+      </c>
+      <c r="C50" t="s">
+        <v>549</v>
+      </c>
+      <c r="D50" t="s">
+        <v>292</v>
+      </c>
+      <c r="E50"/>
+      <c r="F50" t="s">
+        <v>294</v>
+      </c>
+      <c r="G50" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+      <c r="O50" t="s">
+        <v>295</v>
+      </c>
+      <c r="P50" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q50"/>
+      <c r="R50"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>508</v>
+      </c>
+      <c r="B51" t="s">
+        <v>550</v>
+      </c>
+      <c r="C51" t="s">
+        <v>550</v>
+      </c>
+      <c r="D51" t="s">
+        <v>335</v>
+      </c>
+      <c r="E51"/>
+      <c r="F51" t="s">
+        <v>337</v>
+      </c>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+      <c r="O51"/>
+      <c r="P51" t="s">
+        <v>336</v>
+      </c>
+      <c r="Q51"/>
+      <c r="R51"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>509</v>
+      </c>
+      <c r="B52" t="s">
+        <v>551</v>
+      </c>
+      <c r="C52" t="s">
+        <v>551</v>
+      </c>
+      <c r="D52" t="s">
+        <v>338</v>
+      </c>
+      <c r="E52"/>
+      <c r="F52" t="s">
+        <v>340</v>
+      </c>
+      <c r="G52" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="H52" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="I52" t="s">
+        <v>657</v>
+      </c>
+      <c r="J52" t="n">
+        <v>44010.0</v>
+      </c>
+      <c r="K52" t="n">
+        <v>44010.0</v>
+      </c>
+      <c r="L52" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M52" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="N52"/>
+      <c r="O52" t="s">
+        <v>342</v>
+      </c>
+      <c r="P52" t="s">
+        <v>339</v>
+      </c>
+      <c r="Q52"/>
+      <c r="R52" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>510</v>
+      </c>
+      <c r="B53" t="s">
+        <v>552</v>
+      </c>
+      <c r="C53" t="s">
+        <v>552</v>
+      </c>
+      <c r="D53" t="s">
+        <v>594</v>
+      </c>
+      <c r="E53"/>
+      <c r="F53" t="s">
+        <v>652</v>
+      </c>
+      <c r="G53" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="H53" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="I53" t="s">
+        <v>657</v>
+      </c>
+      <c r="J53" t="n">
+        <v>50562.0</v>
+      </c>
+      <c r="K53"/>
+      <c r="L53" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="M53" t="n">
+        <v>106.0</v>
+      </c>
+      <c r="N53" t="n">
+        <v>450.0</v>
+      </c>
+      <c r="O53" t="s">
+        <v>702</v>
+      </c>
+      <c r="P53" t="s">
+        <v>732</v>
+      </c>
+      <c r="Q53"/>
+      <c r="R53" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>511</v>
+      </c>
+      <c r="B54" t="s">
+        <v>553</v>
+      </c>
+      <c r="C54" t="s">
+        <v>553</v>
+      </c>
+      <c r="D54" t="s">
+        <v>595</v>
+      </c>
+      <c r="E54"/>
+      <c r="F54" t="s">
+        <v>653</v>
+      </c>
+      <c r="G54" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H54" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+      <c r="N54"/>
+      <c r="O54"/>
+      <c r="P54" t="s">
+        <v>733</v>
+      </c>
+      <c r="Q54"/>
+      <c r="R54"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>512</v>
+      </c>
+      <c r="B55" t="s">
+        <v>554</v>
+      </c>
+      <c r="C55" t="s">
+        <v>554</v>
+      </c>
+      <c r="D55" t="s">
+        <v>596</v>
+      </c>
+      <c r="E55" t="s">
+        <v>607</v>
+      </c>
+      <c r="F55" t="s">
+        <v>654</v>
+      </c>
+      <c r="G55" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="H55" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="I55" t="s">
+        <v>657</v>
+      </c>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="M55"/>
+      <c r="N55"/>
+      <c r="O55"/>
+      <c r="P55"/>
+      <c r="Q55"/>
+      <c r="R55" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>513</v>
+      </c>
+      <c r="B56" t="s">
+        <v>555</v>
+      </c>
+      <c r="C56" t="s">
+        <v>555</v>
+      </c>
+      <c r="D56" t="s">
+        <v>420</v>
+      </c>
+      <c r="E56"/>
+      <c r="F56" t="s">
+        <v>422</v>
+      </c>
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="M56"/>
+      <c r="N56"/>
+      <c r="O56" t="s">
+        <v>423</v>
+      </c>
+      <c r="P56" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q56"/>
+      <c r="R56"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>514</v>
+      </c>
+      <c r="B57" t="s">
+        <v>556</v>
+      </c>
+      <c r="C57" t="s">
+        <v>556</v>
+      </c>
+      <c r="D57" t="s">
+        <v>597</v>
+      </c>
+      <c r="E57"/>
+      <c r="F57" t="s">
+        <v>655</v>
+      </c>
+      <c r="G57"/>
+      <c r="H57"/>
+      <c r="I57"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="M57"/>
+      <c r="N57"/>
+      <c r="O57"/>
+      <c r="P57" t="s">
+        <v>734</v>
+      </c>
+      <c r="Q57"/>
+      <c r="R57"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>515</v>
+      </c>
+      <c r="B58" t="s">
+        <v>557</v>
+      </c>
+      <c r="C58" t="s">
+        <v>557</v>
+      </c>
+      <c r="D58" t="s">
+        <v>435</v>
+      </c>
+      <c r="E58"/>
+      <c r="F58" t="s">
+        <v>436</v>
+      </c>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58"/>
+      <c r="J58"/>
+      <c r="K58"/>
+      <c r="L58"/>
+      <c r="M58"/>
+      <c r="N58"/>
+      <c r="O58"/>
+      <c r="P58"/>
+      <c r="Q58"/>
+      <c r="R58"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>516</v>
+      </c>
+      <c r="B59" t="s">
+        <v>558</v>
+      </c>
+      <c r="C59" t="s">
+        <v>558</v>
+      </c>
+      <c r="D59" t="s">
+        <v>437</v>
+      </c>
+      <c r="E59"/>
+      <c r="F59" t="s">
+        <v>439</v>
+      </c>
+      <c r="G59" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="H59"/>
+      <c r="I59"/>
+      <c r="J59"/>
+      <c r="K59"/>
+      <c r="L59"/>
+      <c r="M59"/>
+      <c r="N59"/>
+      <c r="O59" t="s">
+        <v>441</v>
+      </c>
+      <c r="P59" t="s">
+        <v>438</v>
+      </c>
+      <c r="Q59"/>
+      <c r="R59"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Proper formatting of description initiatives for output
</commit_message>
<xml_diff>
--- a/dat/synchros-initiatives.xlsx
+++ b/dat/synchros-initiatives.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12090" yWindow="0" windowWidth="20880" windowHeight="7995" tabRatio="500"/>
+    <workbookView xWindow="13950" yWindow="0" windowWidth="20880" windowHeight="7995" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="747">
   <si>
     <t>A consortium of agricultural cohort studies</t>
   </si>
@@ -1401,6 +1401,9 @@
     <t>n_countries</t>
   </si>
   <si>
+    <t>initiative</t>
+  </si>
+  <si>
     <t>age_range</t>
   </si>
   <si>
@@ -1698,9 +1701,9 @@
     <t>The objective of AGRICOH is to support and mantain collaboration and data sharing/pooling to research the association between agricultural exposures and different health outcomes, with emphasis on associations that involve rare exposures and/or health outcomes, and for which data pooling represents a significant gain in statistical power compared to analysis of individual cohorts.</t>
   </si>
   <si>
-    <t>&lt;p&gt;The objective of the ATHLOS Project is to achieve a better understanding of ageing by identifying patterns of healthy ageing pathways or trajectories, the determinants of those patterns, the critical points in time when changes in trajectories are produced, and to propose timely clinical and public health interventions to optimize healthy ageing. Moreover, a new definition of 'old age' based on many characteristics rather than just the classical chronological definition of age will be used for calculating projections in each specific population and guide policy recommendations. To do so, the Consortium will create a harmonised dataset with over 400,000 individuals collated from existing longitudinal studies of ageing and including information on physical and mental health, biomarkers, life style habits, social environment and participation, among others.&lt;/p&gt;
-&lt;p&gt;ATHLOS is a five-year project funded by the European Union's Horizon 2020 Research and Innovation Programme under grant agreement number 635316.&lt;/p&gt;
-&lt;p&gt;The Consortium is coordinated by Dr Josep Maria Haro (Parc Sanitari Sant Joan de Déu) and consists of 14 partners from 11 European countries.&lt;/p&gt;</t>
+    <t>The objective of the ATHLOS Project is to achieve a better understanding of ageing by identifying patterns of healthy ageing pathways or trajectories, the determinants of those patterns, the critical points in time when changes in trajectories are produced, and to propose timely clinical and public health interventions to optimize healthy ageing. Moreover, a new definition of 'old age' based on many characteristics rather than just the classical chronological definition of age will be used for calculating projections in each specific population and guide policy recommendations. To do so, the Consortium will create a harmonised dataset with over 400,000 individuals collated from existing longitudinal studies of ageing and including information on physical and mental health, biomarkers, life style habits, social environment and participation, among others.
+ATHLOS is a five-year project funded by the European Union's Horizon 2020 Research and Innovation Programme under grant agreement number 635316.
+The Consortium is coordinated by Dr Josep Maria Haro (Parc Sanitari Sant Joan de Déu) and consists of 14 partners from 11 European countries.</t>
   </si>
   <si>
     <t>The projects mission is to maximize the use of biosamples, images and data for health research on the prevention, diagnosis and treatment of diseases. For this, these resources are available in a FAIR way: Findable, Accessible, Interoperable and Reusable. This is done in compliance with ethical, legal and privacy demands, and with active participation of donors, citizens and patients.</t>
@@ -1734,25 +1737,23 @@
   </si>
   <si>
     <t>The specific objectives of EUCAN-Connect are:
-* to deliver an open, federated data platform to deposit, curate and analyse cohort (meta)data that meets FAIR principles
-* to create a sustainable framework for long-term collaboration that enables better data-reuse and increased benefit to scientific communities worldwide</t>
-  </si>
-  <si>
-    <t>euCanSHare is a joint EU-Canada project to establish a cross-border data sharing and multi-cohort cardiovascular research platform. 
-Specifically, the project will integrate data infrastructures, IT solutions and data sources from EU, Canada and other countries into a web-based data access system with functionalities for increased efficiency in cardiovascular data-driven research. euCanSHare integrates more than 35 Canadian and European cohorts making up over 1 million records and actively seeks to expand to other regions. 
+- to deliver an open, federated data platform to deposit, curate and analyse cohort (meta)data that meets FAIR principles
+- to create a sustainable framework for long-term collaboration that enables better data-reuse and increased benefit to scientific communities worldwide</t>
+  </si>
+  <si>
+    <t>euCanSHare is a joint EU-Canada project to establish a cross-border data sharing and multi-cohort cardiovascular research platform.
+Specifically, the project will integrate data infrastructures, IT solutions and data sources from EU, Canada and other countries into a web-based data access system with functionalities for increased efficiency in cardiovascular data-driven research. euCanSHare integrates more than 35 Canadian and European cohorts making up over 1 million records and actively seeks to expand to other regions.
 euCanSHare key objectives are: data sharing, knowledge discovery, legal compliance, and community building</t>
   </si>
   <si>
-    <t xml:space="preserve">The Gateway to Global Aging Data (g2aging.org) is a data and information platform developed to facilitate longitudinal and cross-country analyses on aging, especially those using the family of Health and Retirement Studies (HRS) around the world. To further this effort, the Gateway provides searchable metadata, extensive cross-survey documentation, downloadable harmonized microdata with variables standardized across surveys, and graphs and tables that enable users to instantly compare variables of interest over time, across countries, and against macro-level contextual information at no cost.
-</t>
+    <t>The Gateway to Global Aging Data (g2aging.org) is a data and information platform developed to facilitate longitudinal and cross-country analyses on aging, especially those using the family of Health and Retirement Studies (HRS) around the world. To further this effort, the Gateway provides searchable metadata, extensive cross-survey documentation, downloadable harmonized microdata with variables standardized across surveys, and graphs and tables that enable users to instantly compare variables of interest over time, across countries, and against macro-level contextual information at no cost.</t>
   </si>
   <si>
     <t>The aim of GenomEUtwin is to develop novel strategies to maximally utilize the unique features of twin cohorts, including the availability of longitudinal data and sample information about lifestyle and environmental factors, in the characterization of complex traits.</t>
   </si>
   <si>
-    <t xml:space="preserve">The HELIX project is funded to exploit novel tools and methods for characterisation of early-life exposure to a wide range of environmental hazards. These require integration and linkage with data on major child health outcomes, to develop an “Early-Life Exposome” approach.
-Six prospective birth cohort studies (INMA-Spain, RHEA-Greece, MoBa-Norway, EDEN-France, BiB-UK, KANC-Lithuania) are contributing to HELIX as the only realistic and feasible way to obtain the comprehensive, longitudinal, human data needed to build this early-life exposome. These cohorts have already collected large amounts of data as part of national and EU-funded projects. Results will be integrated with data from European cohorts (&gt;300,000 subjects) and registers, to estimate health impacts at the large European scale. This integration of the chemical, physical and molecular environment during critical early-life periods will lead to major improvements in health risk and impact assessments and thus to improved prevention strategies for vulnerable populations.
-</t>
+    <t>The HELIX project is funded to exploit novel tools and methods for characterisation of early-life exposure to a wide range of environmental hazards. These require integration and linkage with data on major child health outcomes, to develop an “Early-Life Exposome” approach.
+Six prospective birth cohort studies (INMA-Spain, RHEA-Greece, MoBa-Norway, EDEN-France, BiB-UK, KANC-Lithuania) are contributing to HELIX as the only realistic and feasible way to obtain the comprehensive, longitudinal, human data needed to build this early-life exposome. These cohorts have already collected large amounts of data as part of national and EU-funded projects. Results will be integrated with data from European cohorts (&gt;300,000 subjects) and registers, to estimate health impacts at the large European scale. This integration of the chemical, physical and molecular environment during critical early-life periods will lead to major improvements in health risk and impact assessments and thus to improved prevention strategies for vulnerable populations.</t>
   </si>
   <si>
     <t>The specific objectives of the initiative are:
@@ -1772,11 +1773,11 @@
 A summary is provided in the publication - 'The International Childhood Cancer Cohort Consortium (I4C): A research platform of prospective cohorts for studying the aetiology of childhood cancers' at the following link - https://onlinelibrary.wiley.com/doi/full/10.1111/ppe.12519</t>
   </si>
   <si>
-    <t>The aim of ICC-dementia is to harmonise centenarian and near-centenarian studies internationally to describe the cognitive and functional profiles of exceptionally old individuals, and ascertain the trajectories of decline and thereby the age-standardised prevalence and incidence of dementia.  The consortium is also interested in the genetic and environmental determinants of dementia-free exceptional longevity.</t>
-  </si>
-  <si>
-    <t>The aim of the IDEAR network is to investigate how determinants in later working life, during the retirement transition, and in early retirement influence for how long older individuals are able to live actively and healthily. 
-This will be done using by state of the art statistical modelling in well-established prospective occupational cohort studies, longitudinal ageing studies and registry data from Sweden, the UK, Finland, France and Denmark. 
+    <t>The aim of ICC-dementia is to harmonise centenarian and near-centenarian studies internationally to describe the cognitive and functional profiles of exceptionally old individuals, and ascertain the trajectories of decline and thereby the age-standardised prevalence and incidence of dementia. The consortium is also interested in the genetic and environmental determinants of dementia-free exceptional longevity.</t>
+  </si>
+  <si>
+    <t>The aim of the IDEAR network is to investigate how determinants in later working life, during the retirement transition, and in early retirement influence for how long older individuals are able to live actively and healthily.
+This will be done using by state of the art statistical modelling in well-established prospective occupational cohort studies, longitudinal ageing studies and registry data from Sweden, the UK, Finland, France and Denmark.
 These studies represent countries in three different welfare regimes and cover up to several decades from mid-life, retirement, early old age, and the beginning of older-old age.</t>
   </si>
   <si>
@@ -1795,9 +1796,9 @@
     <t>The overarching aim of the LIFEPATH project is to understand the determinants of diverging ageing pathways among individuals belonging to different socio-economic groups. This will be achieved via an original study design that integrates social science approaches with biology (including molecular epidemiology), using existing population cohorts and omics measurements (particularly epigenomics).</t>
   </si>
   <si>
-    <t>The objectives of MINDMAP are: 
-1. to harmonize and link data from population registries and cohort studies of mental health ageing in European cities to allow co-analysis of data, based on expertise by Erasmus MC with registry data and McGill University with survey data; 
-2. to develop a conceptual model of mental health in urban settings based on input from experts on mental health from multiple disciplinary perspectives and the integration of results from all work packages on the physical and social environmental, psychosocial, biological and genetic pathways linking the urban environment to mental health; and 
+    <t>The objectives of MINDMAP are:
+1. to harmonize and link data from population registries and cohort studies of mental health ageing in European cities to allow co-analysis of data, based on expertise by Erasmus MC with registry data and McGill University with survey data;
+2. to develop a conceptual model of mental health in urban settings based on input from experts on mental health from multiple disciplinary perspectives and the integration of results from all work packages on the physical and social environmental, psychosocial, biological and genetic pathways linking the urban environment to mental health; and
 3. to develop a methodological framework for the application of advanced causal inference and mediation analysis to study the causal impact of the urban environment on mental health.</t>
   </si>
   <si>
@@ -1807,13 +1808,13 @@
     <t>The overarching concept of OMEGA-NET is to create a network to optimize and integrate occupational, industrial, and population cohorts at the European level, and to provide a foundation for an enhanced evidence base for the identification of health risks and gains related to occupation and employment to foster safe and healthy preventive strategies and policies.
 Research Coordination Objectives and health
 Coordinate and integrate cohorts on occupational health in Europe:
-* Implement an online interactive tool with detailed information on existing cohorts
-* Facilitate work on harmonization of occupational exposure and standardization of health outcome information and new protocols for data collection
-* Promote stakeholder engagement from the start of the project.
+- Implement an online interactive tool with detailed information on existing cohorts
+- Facilitate work on harmonization of occupational exposure and standardization of health outcome information and new protocols for data collection
+- Promote stakeholder engagement from the start of the project.
 Capacity Building Objectives:
-* Connect scientific communities on occupational health in Europe
-* Provide networking and leadership opportunities for early career researchers, as well as researchers from COST Inclusiveness Target Countries
-* Provide training in occupational epidemiology and exposure assessment</t>
+- Connect scientific communities on occupational health in Europe
+- Provide networking and leadership opportunities for early career researchers, as well as researchers from COST Inclusiveness Target Countries
+- Provide training in occupational epidemiology and exposure assessment</t>
   </si>
   <si>
     <t>The aim of ReACH is to provide resources in the form of a comprehensive web-based catalogue and an harmonization platform to optimize and expand the use of Canadian pregnancy and birth cohorts data and biological samples.</t>
@@ -1822,28 +1823,27 @@
     <t>The objective of SAPRIN is to draw together and harmonise a network of South Africa’s health and demographic surveillance sites (HDSS) situated in rural and urban setting, each with a population of at least 100 000 individuals under surveillance.</t>
   </si>
   <si>
-    <t>The Social Inequality in Cancer (SIC) cohort study was established to determine path- ways through which socioeconomic position affects morbidity and mortality, in particular common subtypes of cancer.</t>
+    <t>The Social Inequality in Cancer (SIC) cohort study was established to determine path-ways through which socioeconomic position affects morbidity and mortality, in particular common subtypes of cancer.</t>
   </si>
   <si>
     <t>To establish a genome epidemiological study platform for the research community with a health database and biobank, to investigate the genetic and environmental aetiology of common complex diseases in Koreans and causes of death with long-term follow-up. The ultimate goal of the KoGES was to develop comprehensive and applicable health care guidelines for common complex diseases in Koreans, reduce the burden of chronic diseases and improve the quality of life.</t>
   </si>
   <si>
-    <t xml:space="preserve">To enable the conduct of studies of medication use and outcomes in pregnancy.    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">To maximise the use, value and impact of longitudinal studies to help improve our understanding of key social and biomedical challenges. </t>
-  </si>
-  <si>
-    <t>• harmonize pregnancy and birth cohort data for the 3D, MIREC and SBC studies • establish a collaborative research network on the topic of intra-uterine determinants of child health and development and on perinatal health services in Quebec and Shanghai (China) • establish an infrastructure of knowledge transfer and application between the partners and users of the network leading to updated guidelines, health policies, and knowledge transfer activities in clinical practice • reinforce the strategic positioning of academic and industrial partners in Quebec, China and internationally for providing access to new markets and expertise.</t>
+    <t>- harmonize pregnancy and birth cohort data for the 3D, MIREC and SBC studies
+- establish a collaborative research network on the topic of intra-uterine determinants of child health and development and on perinatal health services in Quebec and Shanghai (China)
+- establish an infrastructure of knowledge transfer and application between the partners and users of the network leading to updated guidelines, health policies, and knowledge transfer activities in clinical practice
+- reinforce the strategic positioning of academic and industrial partners in Quebec, China and internationally for providing access to new markets and expertise.</t>
   </si>
   <si>
     <t>To understand the relationship between genetics, environmental exposures, and the etiology of disease through the establishment of a cohort, or population laboratory.</t>
   </si>
   <si>
-    <t xml:space="preserve">CHANCES aims at combining and integrating ongoing cohort studies in order to produce evidence on ageing-related health characteristics and determinants in Europe and their socio-economic implications.   </t>
-  </si>
-  <si>
-    <t>The scientific goal of ECHO, a research program launched by the National Institutes of Health, is to understand the effects of a broad range of early environmental influences on child health and development. ECHO uses information from existing longitudinal research projects (cohorts), which will include more than 50,000 children from diverse backgrounds across the United States. Together, these cohorts follow participants from before they are born through childhood and adolescence. ECHO also supports a 17-state clinical trials network to test prevention and treatment strategies among children from rural and medically underserved backgrounds. Program Objectives + Improve the health of children and adolescents by conducting observational and interventional research that will inform high-impact programs, policies, and practices. + Institute best practices for conducting Team Science in the 21st century, giving researchers the tools to work collaboratively to improve child health.</t>
+    <t>CHANCES aims at combining and integrating ongoing cohort studies in order to produce evidence on ageing-related health characteristics and determinants in Europe and their socio-economic implications.</t>
+  </si>
+  <si>
+    <t>The scientific goal of ECHO, a research program launched by the National Institutes of Health, is to understand the effects of a broad range of early environmental influences on child health and development. ECHO uses information from existing longitudinal research projects (cohorts), which will include more than 50,000 children from diverse backgrounds across the United States. Together, these cohorts follow participants from before they are born through childhood and adolescence. ECHO also supports a 17-state clinical trials network to test prevention and treatment strategies among children from rural and medically underserved backgrounds. Program Objectives
+- Improve the health of children and adolescents by conducting observational and interventional research that will inform high-impact programs, policies, and practices.
+- Institute best practices for conducting Team Science in the 21st century, giving researchers the tools to work collaboratively to improve child health.</t>
   </si>
   <si>
     <t>Project aims to improve human health through genetic research, and ultimately identify new therapeutic targets and diagnostics for treating numerous diseases. The collaborative nature of the project is exceptional compare to many ongoing studies, and all the partners are working closely together to ensure appropriate transparency, data security and ownership.</t>
@@ -1864,7 +1864,7 @@
     <t>The overall aim of the RECAP preterm Project is to improve the health, development and quality of life of children and adults born very preterm (VPT) or with a very low birth weight (VLBW). This aim will be achieved by combining extensive data from European cohort studies and around the world, which makes it possible to evaluate changes in outcomes over time while providing important information on how the evolution in care and survival of these high risk babies has changed their developmental outcomes and quality of life. We want to develop a better understanding of the origins of VPT/VLBW health and developmental outcomes as well as more effective, evidence-based, personalized interventions and prevention.</t>
   </si>
   <si>
-    <t xml:space="preserve">To identify effective pathways to compressing morbidity and optimising ageing.                                                                                                                         Four key foci, including dementia and cognition, mental health, sensory impairment, and mobility/activity limitations. </t>
+    <t>To identify effective pathways to compressing morbidity and optimising ageing. Four key foci, including dementia and cognition, mental health, sensory impairment, and mobility/activity limitations.</t>
   </si>
   <si>
     <t>Consortium (HAVIC), and cited the following objectives: 1) prospective design, 2) common exposure metrics across cohorts, 3) common health assessment instruments across cohorts, and 4) methods for multisite integration.</t>
@@ -2127,6 +2127,126 @@
   </si>
   <si>
     <t xml:space="preserve">Canada, France        </t>
+  </si>
+  <si>
+    <t>AGRICOH: A consortium of agricultural cohort studies</t>
+  </si>
+  <si>
+    <t>ATHLOS: Ageing Trajectories of Health: Longitudinal Opportunities and Synergies</t>
+  </si>
+  <si>
+    <t>BioSHaRE-EU: Biobank Standardisation and Harmonisation for Research Excellence in the European Union</t>
+  </si>
+  <si>
+    <t>CanPath: Canadian Partnership for Tomorrow’s Health</t>
+  </si>
+  <si>
+    <t>COHORTS.SE: Swedish Cohort Consortium</t>
+  </si>
+  <si>
+    <t>CORDELIA: Collaborative cOhorts Reassembled Data to study mEchanisms and Longterm Incidence of chronic diseAses</t>
+  </si>
+  <si>
+    <t>EClipSE: Epidemiological  Clinicopathological Studies in Europe</t>
+  </si>
+  <si>
+    <t>EPHOR: Exposome Project for Health and Occupational Research</t>
+  </si>
+  <si>
+    <t>HALCyon: Healthy Ageing  across the Life Course</t>
+  </si>
+  <si>
+    <t>HELIX: The Human Early-Life Exposome</t>
+  </si>
+  <si>
+    <t>HeLTI: Healthy Life Trajectories Initiative</t>
+  </si>
+  <si>
+    <t>I3C: International Childhood Cardiovascular Cohort Consortium</t>
+  </si>
+  <si>
+    <t>I4C: International Childhood  Cancer Cohort Consortium</t>
+  </si>
+  <si>
+    <t>ICC-dementia: International  Centenarian Consortium - dementia</t>
+  </si>
+  <si>
+    <t>IDEAR: Integrated Datasets in Europe for Ageing Research</t>
+  </si>
+  <si>
+    <t>IGEMS: Interplay of Genes and Environment across Multiple Studies</t>
+  </si>
+  <si>
+    <t>IHCC: International HundredK+ Cohorts Consortium</t>
+  </si>
+  <si>
+    <t>InterLACE: International Collaboration for a Life Course Approach to  Reproductive Health and Chronic Disease Events</t>
+  </si>
+  <si>
+    <t>LIFEPATH: Lifecourse biological pathways underlying social differences in healthy ageing</t>
+  </si>
+  <si>
+    <t>MINDMAP: Promoting mental well-being and healthy ageing in cities</t>
+  </si>
+  <si>
+    <t>NEAR: National E-lnfrastructure for Aging Research</t>
+  </si>
+  <si>
+    <t>OMEGA-NET: Network on the Coordination and Harmonisation of European Occupational Cohorts project</t>
+  </si>
+  <si>
+    <t>ReACH: Research Advancement through Cohort Cataloguing and Harmonization</t>
+  </si>
+  <si>
+    <t>SAPRIN: South African Population  Research Infrastructure Network</t>
+  </si>
+  <si>
+    <t>SIC: Social Inequality in Cancer cohort study</t>
+  </si>
+  <si>
+    <t>KoGES: The Korean Genome and Epidemiology Study Consortium</t>
+  </si>
+  <si>
+    <t>CLOSER: Cohort and Longitudinal Studies Enhancement Resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPIRIT: Sino-Quebec Perinatal Initiative in Research and Information Technology  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHANCES: Consortium on Health and Ageing: Network of cohorts in Europe and the United States    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FinnGen: Finnish Genome Project </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEMETRIQ: Developing methodologies to reduce inequalities in the determinants of health  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECAP: Research on European Children and adults born preterm  </t>
+  </si>
+  <si>
+    <t>CHICOS: Child Cohort Research Strategy for Europe</t>
+  </si>
+  <si>
+    <t>MeDALL: Mechanisms of the Development of Allergy Project</t>
+  </si>
+  <si>
+    <t>DYNOPTA: Dynamic Analyses to Optimise Ageing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAVIC: The Hand-Arm Vibration International Consortium: Prospective Studies on the Relationship Between Power Tool Exposure and Health Effects     </t>
+  </si>
+  <si>
+    <t>CAPICE: Childhood and Adolescence Psychopathology: unravelling the complex etiology by a large Interdisciplinary Collaboration in Europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIFESPAN: Early-life influences on suicidal ideation, suicide attempts and suicide mortality: a life-course perspective to inform prevention        </t>
+  </si>
+  <si>
+    <t>STOP: Science and Technology in childhood Obesity Policy</t>
+  </si>
+  <si>
+    <t>DYNAHEALTH: Understanding the dynamic determinants of glucose homeostasis and social capability to promote Healthy and active aging</t>
   </si>
   <si>
     <t>0 - 150</t>
@@ -2780,8 +2900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40:H45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7343,6 +7463,9 @@
       <c r="Q1" t="s">
         <v>458</v>
       </c>
+      <c r="R1" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -7356,7 +7479,7 @@
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="F2" t="n">
         <v>30.0</v>
@@ -7365,7 +7488,7 @@
         <v>3.0</v>
       </c>
       <c r="H2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I2" t="n">
         <v>1300000.0</v>
@@ -7381,16 +7504,19 @@
       </c>
       <c r="M2"/>
       <c r="N2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="O2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="P2" t="n">
         <v>12.0</v>
       </c>
       <c r="Q2" t="s">
-        <v>683</v>
+        <v>682</v>
+      </c>
+      <c r="R2" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="3">
@@ -7401,11 +7527,11 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="F3" t="n">
         <v>18.0</v>
@@ -7414,7 +7540,7 @@
         <v>18.0</v>
       </c>
       <c r="H3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I3" t="n">
         <v>411000.0</v>
@@ -7432,31 +7558,34 @@
         <v>180.0</v>
       </c>
       <c r="N3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="O3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="P3" t="n">
         <v>39.0</v>
       </c>
       <c r="Q3" t="s">
-        <v>684</v>
+        <v>683</v>
+      </c>
+      <c r="R3" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B4" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="F4" t="n">
         <v>29.0</v>
@@ -7465,7 +7594,7 @@
         <v>29.0</v>
       </c>
       <c r="H4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I4" t="n">
         <v>700.0</v>
@@ -7481,7 +7610,7 @@
       </c>
       <c r="M4"/>
       <c r="N4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="O4" t="s">
         <v>183</v>
@@ -7490,7 +7619,10 @@
         <v>1.0</v>
       </c>
       <c r="Q4" t="s">
-        <v>685</v>
+        <v>5</v>
+      </c>
+      <c r="R4" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="5">
@@ -7501,11 +7633,11 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="F5" t="n">
         <v>15.0</v>
@@ -7514,7 +7646,7 @@
         <v>8.0</v>
       </c>
       <c r="H5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I5" t="n">
         <v>935227.0</v>
@@ -7528,7 +7660,7 @@
         <v>100.0</v>
       </c>
       <c r="N5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="O5" t="s">
         <v>71</v>
@@ -7537,22 +7669,25 @@
         <v>8.0</v>
       </c>
       <c r="Q5" t="s">
+        <v>684</v>
+      </c>
+      <c r="R5" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B6" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C6" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="F6" t="n">
         <v>7.0</v>
@@ -7561,7 +7696,7 @@
         <v>6.0</v>
       </c>
       <c r="H6" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I6" t="n">
         <v>386641.0</v>
@@ -7579,7 +7714,7 @@
         <v>2840.0</v>
       </c>
       <c r="N6" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="O6" t="s">
         <v>60</v>
@@ -7588,7 +7723,10 @@
         <v>1.0</v>
       </c>
       <c r="Q6" t="s">
-        <v>686</v>
+        <v>685</v>
+      </c>
+      <c r="R6" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="7">
@@ -7599,11 +7737,11 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="F7" t="n">
         <v>40.0</v>
@@ -7612,7 +7750,7 @@
         <v>21.0</v>
       </c>
       <c r="H7" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I7" t="n">
         <v>950000.0</v>
@@ -7630,7 +7768,7 @@
         <v>12.0</v>
       </c>
       <c r="N7" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="O7" t="s">
         <v>88</v>
@@ -7639,22 +7777,25 @@
         <v>1.0</v>
       </c>
       <c r="Q7" t="s">
-        <v>687</v>
+        <v>686</v>
+      </c>
+      <c r="R7" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B8" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C8" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="F8" t="n">
         <v>35.0</v>
@@ -7663,7 +7804,7 @@
         <v>35.0</v>
       </c>
       <c r="H8" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I8" t="n">
         <v>188000.0</v>
@@ -7681,7 +7822,7 @@
         <v>85.0</v>
       </c>
       <c r="N8" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="O8" t="s">
         <v>304</v>
@@ -7690,22 +7831,25 @@
         <v>1.0</v>
       </c>
       <c r="Q8" t="s">
-        <v>688</v>
+        <v>687</v>
+      </c>
+      <c r="R8" t="s">
+        <v>727</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B9" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C9" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F9" t="n">
         <v>3.0</v>
@@ -7714,7 +7858,7 @@
         <v>3.0</v>
       </c>
       <c r="H9" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I9" t="n">
         <v>987.0</v>
@@ -7732,31 +7876,34 @@
         <v>1000.0</v>
       </c>
       <c r="N9" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="O9" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="P9" t="n">
         <v>2.0</v>
       </c>
       <c r="Q9" t="s">
-        <v>689</v>
+        <v>688</v>
+      </c>
+      <c r="R9" t="s">
+        <v>728</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C10" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D10"/>
       <c r="E10" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="F10" t="n">
         <v>40.0</v>
@@ -7765,7 +7912,7 @@
         <v>0.0</v>
       </c>
       <c r="H10" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I10" t="n">
         <v>2.1E7</v>
@@ -7779,29 +7926,32 @@
         <v>0.0</v>
       </c>
       <c r="N10" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="O10" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="P10" t="n">
         <v>12.0</v>
       </c>
-      <c r="Q10"/>
+      <c r="Q10" t="s">
+        <v>689</v>
+      </c>
+      <c r="R10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B11" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C11" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="F11" t="n">
         <v>6.0</v>
@@ -7810,7 +7960,7 @@
         <v>6.0</v>
       </c>
       <c r="H11" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I11" t="n">
         <v>2941.0</v>
@@ -7828,31 +7978,34 @@
         <v>500.0</v>
       </c>
       <c r="N11" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="O11" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="P11" t="n">
         <v>6.0</v>
       </c>
       <c r="Q11" t="s">
-        <v>690</v>
+        <v>409</v>
+      </c>
+      <c r="R11" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B12" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="F12" t="n">
         <v>20.0</v>
@@ -7861,7 +8014,7 @@
         <v>0.0</v>
       </c>
       <c r="H12" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -7871,15 +8024,18 @@
         <v>0.0</v>
       </c>
       <c r="N12" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="O12" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="P12" t="n">
         <v>20.0</v>
       </c>
-      <c r="Q12"/>
+      <c r="Q12" t="s">
+        <v>8</v>
+      </c>
+      <c r="R12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -7892,17 +8048,17 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E13" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F13" t="n">
         <v>32.0</v>
       </c>
       <c r="G13"/>
       <c r="H13" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I13" t="n">
         <v>1000000.0</v>
@@ -7912,31 +8068,34 @@
       <c r="L13"/>
       <c r="M13"/>
       <c r="N13" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="O13" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="P13" t="n">
         <v>15.0</v>
       </c>
-      <c r="Q13"/>
+      <c r="Q13" t="s">
+        <v>9</v>
+      </c>
+      <c r="R13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B14" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C14" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D14" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E14" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="F14" t="n">
         <v>18.0</v>
@@ -7945,7 +8104,7 @@
         <v>10.0</v>
       </c>
       <c r="H14" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I14" t="n">
         <v>351000.0</v>
@@ -7961,16 +8120,19 @@
         <v>37000.0</v>
       </c>
       <c r="N14" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="O14" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="P14" t="n">
         <v>43.0</v>
       </c>
       <c r="Q14" t="s">
-        <v>691</v>
+        <v>510</v>
+      </c>
+      <c r="R14" t="s">
+        <v>730</v>
       </c>
     </row>
     <row r="15">
@@ -7985,7 +8147,7 @@
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="F15" t="n">
         <v>9.0</v>
@@ -7994,7 +8156,7 @@
         <v>9.0</v>
       </c>
       <c r="H15" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I15" t="n">
         <v>1190000.0</v>
@@ -8008,27 +8170,30 @@
       </c>
       <c r="M15"/>
       <c r="N15" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="O15" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="P15" t="n">
         <v>8.0</v>
       </c>
       <c r="Q15" t="s">
-        <v>692</v>
+        <v>11</v>
+      </c>
+      <c r="R15" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B16" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C16" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="s">
@@ -8041,7 +8206,7 @@
         <v>9.0</v>
       </c>
       <c r="H16" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I16" t="n">
         <v>40000.0</v>
@@ -8055,7 +8220,7 @@
       </c>
       <c r="M16"/>
       <c r="N16" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="O16" t="s">
         <v>95</v>
@@ -8064,7 +8229,10 @@
         <v>1.0</v>
       </c>
       <c r="Q16" t="s">
-        <v>693</v>
+        <v>690</v>
+      </c>
+      <c r="R16" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="17">
@@ -8075,13 +8243,13 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="F17" t="n">
         <v>6.0</v>
@@ -8090,7 +8258,7 @@
         <v>6.0</v>
       </c>
       <c r="H17" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I17" t="n">
         <v>32000.0</v>
@@ -8106,31 +8274,34 @@
       </c>
       <c r="M17"/>
       <c r="N17" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="O17" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="P17" t="n">
         <v>6.0</v>
       </c>
       <c r="Q17" t="s">
-        <v>694</v>
+        <v>691</v>
+      </c>
+      <c r="R17" t="s">
+        <v>733</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B18" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C18" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="F18" t="n">
         <v>4.0</v>
@@ -8139,7 +8310,7 @@
         <v>4.0</v>
       </c>
       <c r="H18" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I18" t="n">
         <v>22730.0</v>
@@ -8155,7 +8326,7 @@
         <v>1043.0</v>
       </c>
       <c r="N18" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="O18" t="s">
         <v>166</v>
@@ -8164,6 +8335,9 @@
         <v>4.0</v>
       </c>
       <c r="Q18" t="s">
+        <v>692</v>
+      </c>
+      <c r="R18" t="s">
         <v>174</v>
       </c>
     </row>
@@ -8175,11 +8349,11 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="F19" t="n">
         <v>7.0</v>
@@ -8188,7 +8362,7 @@
         <v>7.0</v>
       </c>
       <c r="H19" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I19" t="n">
         <v>42189.0</v>
@@ -8206,31 +8380,34 @@
         <v>15.0</v>
       </c>
       <c r="N19" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="O19" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="P19" t="n">
         <v>3.0</v>
       </c>
       <c r="Q19" t="s">
-        <v>695</v>
+        <v>693</v>
+      </c>
+      <c r="R19" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B20" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C20" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="F20" t="n">
         <v>6.0</v>
@@ -8239,7 +8416,7 @@
         <v>6.0</v>
       </c>
       <c r="H20" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I20" t="n">
         <v>388120.0</v>
@@ -8255,33 +8432,36 @@
         <v>20.0</v>
       </c>
       <c r="N20" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="O20" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="P20" t="n">
         <v>11.0</v>
       </c>
       <c r="Q20" t="s">
-        <v>696</v>
+        <v>694</v>
+      </c>
+      <c r="R20" t="s">
+        <v>735</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B21" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C21" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D21" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E21" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="F21" t="n">
         <v>18.0</v>
@@ -8290,7 +8470,7 @@
         <v>18.0</v>
       </c>
       <c r="H21" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I21" t="n">
         <v>7960.0</v>
@@ -8302,29 +8482,32 @@
       <c r="L21"/>
       <c r="M21"/>
       <c r="N21" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="O21"/>
       <c r="P21" t="n">
         <v>1.0</v>
       </c>
       <c r="Q21" t="s">
-        <v>697</v>
+        <v>695</v>
+      </c>
+      <c r="R21" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B22" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C22" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="F22" t="n">
         <v>10.0</v>
@@ -8333,7 +8516,7 @@
         <v>6.0</v>
       </c>
       <c r="H22" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I22" t="n">
         <v>5000000.0</v>
@@ -8351,16 +8534,19 @@
         <v>15.0</v>
       </c>
       <c r="N22" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="O22" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="P22" t="n">
         <v>5.0</v>
       </c>
       <c r="Q22" t="s">
-        <v>698</v>
+        <v>696</v>
+      </c>
+      <c r="R22" t="s">
+        <v>737</v>
       </c>
     </row>
     <row r="23">
@@ -8371,11 +8557,11 @@
         <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="F23" t="n">
         <v>18.0</v>
@@ -8384,7 +8570,7 @@
         <v>18.0</v>
       </c>
       <c r="H23" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I23" t="n">
         <v>76233.0</v>
@@ -8402,31 +8588,34 @@
         <v>31.0</v>
       </c>
       <c r="N23" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="O23" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="P23" t="n">
         <v>5.0</v>
       </c>
       <c r="Q23" t="s">
-        <v>699</v>
+        <v>697</v>
+      </c>
+      <c r="R23" t="s">
+        <v>738</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B24" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C24" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F24" t="n">
         <v>67.0</v>
@@ -8435,7 +8624,7 @@
         <v>0.0</v>
       </c>
       <c r="H24" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I24"/>
       <c r="J24"/>
@@ -8447,31 +8636,34 @@
       </c>
       <c r="M24"/>
       <c r="N24" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="O24"/>
       <c r="P24" t="n">
         <v>1.0</v>
       </c>
       <c r="Q24" t="s">
-        <v>683</v>
+        <v>698</v>
+      </c>
+      <c r="R24" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B25" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C25" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="F25" t="n">
         <v>43.0</v>
@@ -8480,7 +8672,7 @@
         <v>43.0</v>
       </c>
       <c r="H25" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I25" t="n">
         <v>1000000.0</v>
@@ -8494,29 +8686,32 @@
         <v>100.0</v>
       </c>
       <c r="N25" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="O25"/>
       <c r="P25" t="n">
         <v>1.0</v>
       </c>
-      <c r="Q25"/>
+      <c r="Q25" t="s">
+        <v>474</v>
+      </c>
+      <c r="R25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B26" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C26" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D26" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="E26" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="F26" t="n">
         <v>26.0</v>
@@ -8525,7 +8720,7 @@
         <v>26.0</v>
       </c>
       <c r="H26" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I26" t="n">
         <v>839666.0</v>
@@ -8543,31 +8738,34 @@
         <v>1300.0</v>
       </c>
       <c r="N26" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="O26" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="P26" t="n">
         <v>11.0</v>
       </c>
       <c r="Q26" t="s">
-        <v>700</v>
+        <v>699</v>
+      </c>
+      <c r="R26" t="s">
+        <v>739</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B27" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
       </c>
       <c r="D27"/>
       <c r="E27" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="F27" t="n">
         <v>18.0</v>
@@ -8576,7 +8774,7 @@
         <v>8.0</v>
       </c>
       <c r="H27" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I27" t="n">
         <v>1941000.0</v>
@@ -8594,16 +8792,19 @@
         <v>270.0</v>
       </c>
       <c r="N27" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="O27" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="P27" t="n">
         <v>9.0</v>
       </c>
       <c r="Q27" t="s">
-        <v>683</v>
+        <v>700</v>
+      </c>
+      <c r="R27" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="28">
@@ -8614,11 +8815,11 @@
         <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="D28"/>
       <c r="E28" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="F28" t="n">
         <v>10.0</v>
@@ -8627,7 +8828,7 @@
         <v>9.0</v>
       </c>
       <c r="H28" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I28" t="n">
         <v>2662777.0</v>
@@ -8643,15 +8844,18 @@
         <v>2560.0</v>
       </c>
       <c r="N28" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="O28" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="P28" t="n">
         <v>9.0</v>
       </c>
       <c r="Q28" t="s">
+        <v>701</v>
+      </c>
+      <c r="R28" t="s">
         <v>78</v>
       </c>
     </row>
@@ -8663,11 +8867,11 @@
         <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D29"/>
       <c r="E29" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="F29" t="n">
         <v>15.0</v>
@@ -8676,7 +8880,7 @@
         <v>0.0</v>
       </c>
       <c r="H29" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I29" t="n">
         <v>190268.0</v>
@@ -8690,7 +8894,7 @@
       <c r="L29"/>
       <c r="M29"/>
       <c r="N29" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="O29" t="s">
         <v>88</v>
@@ -8699,31 +8903,34 @@
         <v>1.0</v>
       </c>
       <c r="Q29" t="s">
-        <v>701</v>
+        <v>702</v>
+      </c>
+      <c r="R29" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B30" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C30" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="D30" t="s">
         <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="F30"/>
       <c r="G30" t="n">
         <v>0.0</v>
       </c>
       <c r="H30" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I30"/>
       <c r="J30"/>
@@ -8731,29 +8938,32 @@
       <c r="L30"/>
       <c r="M30"/>
       <c r="N30" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="O30"/>
       <c r="P30" t="n">
         <v>1.0</v>
       </c>
-      <c r="Q30"/>
+      <c r="Q30" t="s">
+        <v>703</v>
+      </c>
+      <c r="R30"/>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B31" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C31" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D31" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E31" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="F31" t="n">
         <v>27.0</v>
@@ -8762,7 +8972,7 @@
         <v>27.0</v>
       </c>
       <c r="H31" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I31" t="n">
         <v>89889.0</v>
@@ -8776,31 +8986,34 @@
       </c>
       <c r="M31"/>
       <c r="N31" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="O31" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="P31" t="n">
         <v>12.0</v>
       </c>
       <c r="Q31" t="s">
-        <v>702</v>
+        <v>704</v>
+      </c>
+      <c r="R31" t="s">
+        <v>741</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B32" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C32" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D32"/>
       <c r="E32" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="F32" t="n">
         <v>5.0</v>
@@ -8809,7 +9022,7 @@
         <v>3.0</v>
       </c>
       <c r="H32" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I32" t="n">
         <v>315000.0</v>
@@ -8827,7 +9040,7 @@
         <v>52.0</v>
       </c>
       <c r="N32" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="O32" t="s">
         <v>237</v>
@@ -8836,22 +9049,25 @@
         <v>1.0</v>
       </c>
       <c r="Q32" t="s">
-        <v>685</v>
+        <v>705</v>
+      </c>
+      <c r="R32" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B33" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C33" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="D33"/>
       <c r="E33" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="F33" t="n">
         <v>7.0</v>
@@ -8860,7 +9076,7 @@
         <v>7.0</v>
       </c>
       <c r="H33" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I33" t="n">
         <v>83006.0</v>
@@ -8878,7 +9094,7 @@
         <v>28.0</v>
       </c>
       <c r="N33" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="O33" t="s">
         <v>344</v>
@@ -8887,29 +9103,32 @@
         <v>1.0</v>
       </c>
       <c r="Q33" t="s">
-        <v>703</v>
+        <v>706</v>
+      </c>
+      <c r="R33" t="s">
+        <v>742</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B34" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C34" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D34"/>
       <c r="E34" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="F34" t="n">
         <v>6.0</v>
       </c>
       <c r="G34"/>
       <c r="H34" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I34" t="n">
         <v>245000.0</v>
@@ -8919,13 +9138,16 @@
       <c r="L34"/>
       <c r="M34"/>
       <c r="N34" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="O34" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P34"/>
-      <c r="Q34"/>
+      <c r="Q34" t="s">
+        <v>707</v>
+      </c>
+      <c r="R34"/>
     </row>
     <row r="35">
       <c r="A35" t="s">
@@ -8935,11 +9157,11 @@
         <v>47</v>
       </c>
       <c r="C35" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D35"/>
       <c r="E35" t="s">
-        <v>588</v>
+        <v>49</v>
       </c>
       <c r="F35" t="n">
         <v>11.0</v>
@@ -8954,13 +9176,16 @@
       <c r="L35"/>
       <c r="M35"/>
       <c r="N35" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="O35" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="P35"/>
-      <c r="Q35"/>
+      <c r="Q35" t="s">
+        <v>528</v>
+      </c>
+      <c r="R35"/>
     </row>
     <row r="36">
       <c r="A36" t="s">
@@ -8970,11 +9195,11 @@
         <v>93</v>
       </c>
       <c r="C36" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D36"/>
       <c r="E36" t="s">
-        <v>589</v>
+        <v>96</v>
       </c>
       <c r="F36" t="n">
         <v>8.0</v>
@@ -8991,26 +9216,29 @@
         <v>8.0</v>
       </c>
       <c r="N36" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="O36" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="P36"/>
-      <c r="Q36"/>
+      <c r="Q36" t="s">
+        <v>708</v>
+      </c>
+      <c r="R36"/>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B37" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C37" t="s">
         <v>106</v>
       </c>
       <c r="D37" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E37" t="s">
         <v>108</v>
@@ -9022,7 +9250,7 @@
         <v>4.0</v>
       </c>
       <c r="H37" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I37"/>
       <c r="J37"/>
@@ -9032,7 +9260,10 @@
       <c r="N37"/>
       <c r="O37"/>
       <c r="P37"/>
-      <c r="Q37"/>
+      <c r="Q37" t="s">
+        <v>106</v>
+      </c>
+      <c r="R37"/>
     </row>
     <row r="38">
       <c r="A38" t="s">
@@ -9042,11 +9273,11 @@
         <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D38"/>
       <c r="E38" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F38" t="n">
         <v>4.0</v>
@@ -9061,25 +9292,28 @@
       <c r="L38"/>
       <c r="M38"/>
       <c r="N38" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="O38" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="P38"/>
-      <c r="Q38"/>
+      <c r="Q38" t="s">
+        <v>709</v>
+      </c>
+      <c r="R38"/>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B39"/>
       <c r="C39" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D39"/>
       <c r="E39" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F39" t="n">
         <v>29.0</v>
@@ -9088,7 +9322,7 @@
         <v>24.0</v>
       </c>
       <c r="H39" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I39" t="n">
         <v>1221985.0</v>
@@ -9104,29 +9338,32 @@
         <v>600.0</v>
       </c>
       <c r="N39" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="O39" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="P39"/>
       <c r="Q39" t="s">
-        <v>704</v>
+        <v>483</v>
+      </c>
+      <c r="R39" t="s">
+        <v>743</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B40" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C40" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D40"/>
       <c r="E40" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F40" t="n">
         <v>14.0</v>
@@ -9135,7 +9372,7 @@
         <v>14.0</v>
       </c>
       <c r="H40" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I40"/>
       <c r="J40"/>
@@ -9147,29 +9384,32 @@
         <v>323.0</v>
       </c>
       <c r="N40" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="O40" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="P40"/>
       <c r="Q40" t="s">
+        <v>710</v>
+      </c>
+      <c r="R40" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B41" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C41" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D41"/>
       <c r="E41" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F41" t="n">
         <v>84.0</v>
@@ -9184,27 +9424,30 @@
       <c r="L41"/>
       <c r="M41"/>
       <c r="N41" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="O41" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="P41"/>
-      <c r="Q41"/>
+      <c r="Q41" t="s">
+        <v>532</v>
+      </c>
+      <c r="R41"/>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B42" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C42" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D42"/>
       <c r="E42" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F42"/>
       <c r="G42"/>
@@ -9215,25 +9458,28 @@
       <c r="L42"/>
       <c r="M42"/>
       <c r="N42" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="O42" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="P42"/>
-      <c r="Q42"/>
+      <c r="Q42" t="s">
+        <v>711</v>
+      </c>
+      <c r="R42"/>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B43"/>
       <c r="C43" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="D43"/>
       <c r="E43" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F43"/>
       <c r="G43"/>
@@ -9246,34 +9492,37 @@
       <c r="L43"/>
       <c r="M43"/>
       <c r="N43" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="O43" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="P43"/>
-      <c r="Q43"/>
+      <c r="Q43" t="s">
+        <v>487</v>
+      </c>
+      <c r="R43"/>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B44" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C44" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="D44" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E44" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F44"/>
       <c r="G44"/>
       <c r="H44" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I44"/>
       <c r="J44"/>
@@ -9283,24 +9532,27 @@
       <c r="N44"/>
       <c r="O44"/>
       <c r="P44"/>
-      <c r="Q44"/>
+      <c r="Q44" t="s">
+        <v>712</v>
+      </c>
+      <c r="R44"/>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B45"/>
       <c r="C45" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="D45"/>
       <c r="E45" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F45"/>
       <c r="G45"/>
       <c r="H45" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I45"/>
       <c r="J45"/>
@@ -9308,13 +9560,16 @@
       <c r="L45"/>
       <c r="M45"/>
       <c r="N45" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="O45" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="P45"/>
-      <c r="Q45"/>
+      <c r="Q45" t="s">
+        <v>489</v>
+      </c>
+      <c r="R45"/>
     </row>
     <row r="46">
       <c r="A46" t="s">
@@ -9335,7 +9590,7 @@
         <v>19.0</v>
       </c>
       <c r="H46" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I46" t="n">
         <v>250000.0</v>
@@ -9349,21 +9604,24 @@
       </c>
       <c r="O46"/>
       <c r="P46"/>
-      <c r="Q46"/>
+      <c r="Q46" t="s">
+        <v>252</v>
+      </c>
+      <c r="R46"/>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B47" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C47" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D47"/>
       <c r="E47" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F47" t="n">
         <v>6.0</v>
@@ -9372,7 +9630,7 @@
         <v>6.0</v>
       </c>
       <c r="H47" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I47" t="n">
         <v>136128.0</v>
@@ -9386,31 +9644,34 @@
       <c r="L47"/>
       <c r="M47"/>
       <c r="N47" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="O47" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="P47"/>
       <c r="Q47" t="s">
+        <v>535</v>
+      </c>
+      <c r="R47" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B48" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C48" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D48" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="E48" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F48" t="n">
         <v>20.0</v>
@@ -9423,11 +9684,14 @@
       <c r="L48"/>
       <c r="M48"/>
       <c r="N48" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="O48"/>
       <c r="P48"/>
-      <c r="Q48"/>
+      <c r="Q48" t="s">
+        <v>713</v>
+      </c>
+      <c r="R48"/>
     </row>
     <row r="49">
       <c r="A49" t="s">
@@ -9440,7 +9704,7 @@
         <v>280</v>
       </c>
       <c r="D49" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E49" t="s">
         <v>282</v>
@@ -9452,7 +9716,7 @@
         <v>69.0</v>
       </c>
       <c r="H49" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I49" t="n">
         <v>320000.0</v>
@@ -9473,18 +9737,21 @@
       <c r="O49"/>
       <c r="P49"/>
       <c r="Q49" t="s">
+        <v>280</v>
+      </c>
+      <c r="R49" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B50" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C50" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D50"/>
       <c r="E50" t="s">
@@ -9507,17 +9774,20 @@
         <v>293</v>
       </c>
       <c r="P50"/>
-      <c r="Q50"/>
+      <c r="Q50" t="s">
+        <v>714</v>
+      </c>
+      <c r="R50"/>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B51" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C51" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="D51"/>
       <c r="E51" t="s">
@@ -9536,17 +9806,20 @@
         <v>336</v>
       </c>
       <c r="P51"/>
-      <c r="Q51"/>
+      <c r="Q51" t="s">
+        <v>335</v>
+      </c>
+      <c r="R51"/>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B52" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C52" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D52"/>
       <c r="E52" t="s">
@@ -9559,7 +9832,7 @@
         <v>13.0</v>
       </c>
       <c r="H52" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I52" t="n">
         <v>44010.0</v>
@@ -9582,22 +9855,25 @@
       </c>
       <c r="P52"/>
       <c r="Q52" t="s">
-        <v>705</v>
+        <v>715</v>
+      </c>
+      <c r="R52" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B53" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C53" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="D53"/>
       <c r="E53" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F53" t="n">
         <v>9.0</v>
@@ -9606,7 +9882,7 @@
         <v>9.0</v>
       </c>
       <c r="H53" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I53" t="n">
         <v>50562.0</v>
@@ -9622,29 +9898,32 @@
         <v>450.0</v>
       </c>
       <c r="N53" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="O53" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="P53"/>
       <c r="Q53" t="s">
-        <v>706</v>
+        <v>716</v>
+      </c>
+      <c r="R53" t="s">
+        <v>745</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B54" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C54" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="D54"/>
       <c r="E54" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F54" t="n">
         <v>6.0</v>
@@ -9660,26 +9939,29 @@
       <c r="M54"/>
       <c r="N54"/>
       <c r="O54" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="P54"/>
-      <c r="Q54"/>
+      <c r="Q54" t="s">
+        <v>717</v>
+      </c>
+      <c r="R54"/>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B55" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C55" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="D55" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="E55" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F55" t="n">
         <v>10.0</v>
@@ -9688,7 +9970,7 @@
         <v>10.0</v>
       </c>
       <c r="H55" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I55"/>
       <c r="J55"/>
@@ -9701,18 +9983,21 @@
       <c r="O55"/>
       <c r="P55"/>
       <c r="Q55" t="s">
-        <v>707</v>
+        <v>542</v>
+      </c>
+      <c r="R55" t="s">
+        <v>746</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B56" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C56" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D56"/>
       <c r="E56" t="s">
@@ -9733,21 +10018,24 @@
         <v>421</v>
       </c>
       <c r="P56"/>
-      <c r="Q56"/>
+      <c r="Q56" t="s">
+        <v>718</v>
+      </c>
+      <c r="R56"/>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B57" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C57" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="D57"/>
       <c r="E57" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F57"/>
       <c r="G57"/>
@@ -9759,20 +10047,23 @@
       <c r="M57"/>
       <c r="N57"/>
       <c r="O57" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="P57"/>
-      <c r="Q57"/>
+      <c r="Q57" t="s">
+        <v>719</v>
+      </c>
+      <c r="R57"/>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B58" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C58" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D58"/>
       <c r="E58" t="s">
@@ -9789,17 +10080,20 @@
       <c r="N58"/>
       <c r="O58"/>
       <c r="P58"/>
-      <c r="Q58"/>
+      <c r="Q58" t="s">
+        <v>720</v>
+      </c>
+      <c r="R58"/>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B59" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C59" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D59"/>
       <c r="E59" t="s">
@@ -9822,7 +10116,10 @@
         <v>438</v>
       </c>
       <c r="P59"/>
-      <c r="Q59"/>
+      <c r="Q59" t="s">
+        <v>721</v>
+      </c>
+      <c r="R59"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Standardizes data in Table 1 used to complete information of countries / regions
</commit_message>
<xml_diff>
--- a/dat/synchros-initiatives.xlsx
+++ b/dat/synchros-initiatives.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14880" yWindow="0" windowWidth="20880" windowHeight="7995" tabRatio="500"/>
+    <workbookView xWindow="18600" yWindow="0" windowWidth="20880" windowHeight="7995" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="752">
   <si>
     <t>A consortium of agricultural cohort studies</t>
   </si>
@@ -1686,7 +1686,7 @@
     <t>Principally Canada</t>
   </si>
   <si>
-    <t>American, European, Asian countries</t>
+    <t xml:space="preserve">Asia  </t>
   </si>
   <si>
     <t xml:space="preserve">Europe (27 countries)  </t>
@@ -1695,10 +1695,7 @@
     <t xml:space="preserve">Europe  </t>
   </si>
   <si>
-    <t>Australia, 15 European countries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USA, Europe </t>
+    <t xml:space="preserve">USA and Europe </t>
   </si>
   <si>
     <t>The objective of AGRICOH is to support and mantain collaboration and data sharing/pooling to research the association between agricultural exposures and different health outcomes, with emphasis on associations that involve rare exposures and/or health outcomes, and for which data pooling represents a significant gain in statistical power compared to analysis of individual cohorts.</t>
@@ -2090,46 +2087,40 @@
     <t>Argentina, Australia, Belgium, Brazil, Canada, Chile, Croatia, Egypt, Estonia, Germany, Greece, Hungary</t>
   </si>
   <si>
-    <t xml:space="preserve">South Korea, Vietnam, Cambodia, Japan, China </t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States of America    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">United Kingdom </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canada, China   </t>
-  </si>
-  <si>
-    <t>Bangladesh, Japan, Taiwan, South Korea, China, India, Singapore, Iran, Mongolia, Singapore Malaysia,, the United States</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United Kingdom, The Netherlands, Germany, France, Denmark, Greece, Finland, Norway, Sweden, United States   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finland </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asia  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tohoku (region of Japan) </t>
-  </si>
-  <si>
-    <t>China, Ghana, India, Mexico, the Russian Federation, South Africa, England, USA, Austria, Belgium, Denmark, France, Germany, Greece, Italy, Switzerland, The Netherlands, Spain, Sweden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Australia </t>
-  </si>
-  <si>
-    <t xml:space="preserve">US, Sweden, Finland      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canada, France        </t>
+    <t>Canada, China</t>
+  </si>
+  <si>
+    <t>Bangladesh, Japan, Taiwan, South Korea, China, India, Singapore, Iran, Mongolia, Singapore, Malaysia, United States</t>
+  </si>
+  <si>
+    <t>United Kingdom, Netherlands, Germany, France, Denmark, Greece, Finland, Norway, Sweden, United States</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>China, Ghana, India, Mexico, Russia, South Africa, United Kingdom, United States, Austria, Belgium, Denmark, France, Germany, Greece, Italy, Switzerland, Netherlands, Spain, Sweden</t>
+  </si>
+  <si>
+    <t>Belgium, Czechia, Denmark, Faroe Islands, Finland, France, Germany, Greece, Ireland, Italy, Lithuania, Netherlands, Norway, Poland, Portugal, Slovakia, Spain, Sweden, Switzerland, Ukraine, United Kingdom</t>
+  </si>
+  <si>
+    <t>Norway, Finland, Sweden, United Kingdom, Netherlands, France, Spain, Italy</t>
+  </si>
+  <si>
+    <t>Spain, Sweden, United Kingdom, Denmark, Norway, France, Germany, Netherlands, Greece, Italy</t>
+  </si>
+  <si>
+    <t>United States, Sweden, Finland</t>
+  </si>
+  <si>
+    <t>Italy, Netherlands, United Kingdom, Sweden</t>
+  </si>
+  <si>
+    <t>Canada, France</t>
+  </si>
+  <si>
+    <t>Finland, Denmark, Netherlands, Germany, Spain, Belgium, Italy, Poland</t>
   </si>
   <si>
     <t>AGRICOH: A consortium of agricultural cohort studies</t>
@@ -2273,9 +2264,15 @@
     <t>65 - 150</t>
   </si>
   <si>
+    <t xml:space="preserve">To be determined. The project has not begun yet. </t>
+  </si>
+  <si>
     <t>65 - 85</t>
   </si>
   <si>
+    <t xml:space="preserve">To Be Determined   </t>
+  </si>
+  <si>
     <t>45+</t>
   </si>
   <si>
@@ -2303,6 +2300,9 @@
     <t>14 - 103</t>
   </si>
   <si>
+    <t xml:space="preserve">This depends on the consortium in question </t>
+  </si>
+  <si>
     <t>30 - 75</t>
   </si>
   <si>
@@ -2315,7 +2315,19 @@
     <t>20 - 93</t>
   </si>
   <si>
+    <t xml:space="preserve">It depends on the project </t>
+  </si>
+  <si>
     <t>40+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all ages  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Undefined  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All (Fetus to old ages) </t>
   </si>
   <si>
     <t>0 - 17</t>
@@ -7485,7 +7497,7 @@
       </c>
       <c r="D2"/>
       <c r="E2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F2" t="n">
         <v>30.0</v>
@@ -7494,7 +7506,7 @@
         <v>3.0</v>
       </c>
       <c r="H2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I2" t="n">
         <v>1300000.0</v>
@@ -7510,22 +7522,22 @@
       </c>
       <c r="M2"/>
       <c r="N2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="O2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="P2" t="n">
         <v>12.0</v>
       </c>
       <c r="Q2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="R2" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="S2" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
     </row>
     <row r="3">
@@ -7540,7 +7552,7 @@
       </c>
       <c r="D3"/>
       <c r="E3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F3" t="n">
         <v>18.0</v>
@@ -7549,7 +7561,7 @@
         <v>18.0</v>
       </c>
       <c r="H3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I3" t="n">
         <v>411000.0</v>
@@ -7567,22 +7579,22 @@
         <v>180.0</v>
       </c>
       <c r="N3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="O3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="P3" t="n">
         <v>39.0</v>
       </c>
       <c r="Q3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="R3" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="S3" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
     </row>
     <row r="4">
@@ -7597,7 +7609,7 @@
       </c>
       <c r="D4"/>
       <c r="E4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F4" t="n">
         <v>29.0</v>
@@ -7606,7 +7618,7 @@
         <v>29.0</v>
       </c>
       <c r="H4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I4" t="n">
         <v>700.0</v>
@@ -7622,7 +7634,7 @@
       </c>
       <c r="M4"/>
       <c r="N4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="O4" t="s">
         <v>183</v>
@@ -7637,7 +7649,7 @@
         <v>5</v>
       </c>
       <c r="S4" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
     </row>
     <row r="5">
@@ -7652,7 +7664,7 @@
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F5" t="n">
         <v>15.0</v>
@@ -7661,7 +7673,7 @@
         <v>8.0</v>
       </c>
       <c r="H5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I5" t="n">
         <v>935227.0</v>
@@ -7675,7 +7687,7 @@
         <v>100.0</v>
       </c>
       <c r="N5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="O5" t="s">
         <v>71</v>
@@ -7687,7 +7699,7 @@
         <v>71</v>
       </c>
       <c r="R5" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="S5" t="s">
         <v>174</v>
@@ -7705,7 +7717,7 @@
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F6" t="n">
         <v>7.0</v>
@@ -7714,7 +7726,7 @@
         <v>6.0</v>
       </c>
       <c r="H6" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I6" t="n">
         <v>386641.0</v>
@@ -7732,7 +7744,7 @@
         <v>2840.0</v>
       </c>
       <c r="N6" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="O6" t="s">
         <v>60</v>
@@ -7744,10 +7756,10 @@
         <v>60</v>
       </c>
       <c r="R6" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="S6" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
     </row>
     <row r="7">
@@ -7762,7 +7774,7 @@
       </c>
       <c r="D7"/>
       <c r="E7" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F7" t="n">
         <v>40.0</v>
@@ -7771,7 +7783,7 @@
         <v>21.0</v>
       </c>
       <c r="H7" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I7" t="n">
         <v>950000.0</v>
@@ -7789,7 +7801,7 @@
         <v>12.0</v>
       </c>
       <c r="N7" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="O7" t="s">
         <v>88</v>
@@ -7801,10 +7813,10 @@
         <v>88</v>
       </c>
       <c r="R7" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="S7" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
     </row>
     <row r="8">
@@ -7819,7 +7831,7 @@
       </c>
       <c r="D8"/>
       <c r="E8" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F8" t="n">
         <v>35.0</v>
@@ -7828,7 +7840,7 @@
         <v>35.0</v>
       </c>
       <c r="H8" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I8" t="n">
         <v>188000.0</v>
@@ -7846,7 +7858,7 @@
         <v>85.0</v>
       </c>
       <c r="N8" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="O8" t="s">
         <v>304</v>
@@ -7858,10 +7870,10 @@
         <v>304</v>
       </c>
       <c r="R8" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="S8" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
     </row>
     <row r="9">
@@ -7876,7 +7888,7 @@
       </c>
       <c r="D9"/>
       <c r="E9" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F9" t="n">
         <v>3.0</v>
@@ -7885,7 +7897,7 @@
         <v>3.0</v>
       </c>
       <c r="H9" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I9" t="n">
         <v>987.0</v>
@@ -7903,22 +7915,22 @@
         <v>1000.0</v>
       </c>
       <c r="N9" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="O9" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="P9" t="n">
         <v>2.0</v>
       </c>
       <c r="Q9" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="R9" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="S9" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
     </row>
     <row r="10">
@@ -7933,7 +7945,7 @@
       </c>
       <c r="D10"/>
       <c r="E10" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F10" t="n">
         <v>40.0</v>
@@ -7942,7 +7954,7 @@
         <v>0.0</v>
       </c>
       <c r="H10" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I10" t="n">
         <v>2.1E7</v>
@@ -7956,21 +7968,23 @@
         <v>0.0</v>
       </c>
       <c r="N10" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="O10" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="P10" t="n">
         <v>12.0</v>
       </c>
       <c r="Q10" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="R10" t="s">
-        <v>690</v>
-      </c>
-      <c r="S10"/>
+        <v>687</v>
+      </c>
+      <c r="S10" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -7984,7 +7998,7 @@
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F11" t="n">
         <v>6.0</v>
@@ -7993,7 +8007,7 @@
         <v>6.0</v>
       </c>
       <c r="H11" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I11" t="n">
         <v>2941.0</v>
@@ -8011,22 +8025,22 @@
         <v>500.0</v>
       </c>
       <c r="N11" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="O11" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="P11" t="n">
         <v>6.0</v>
       </c>
       <c r="Q11" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="R11" t="s">
         <v>409</v>
       </c>
       <c r="S11" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="12">
@@ -8041,7 +8055,7 @@
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F12" t="n">
         <v>20.0</v>
@@ -8050,7 +8064,7 @@
         <v>0.0</v>
       </c>
       <c r="H12" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -8060,21 +8074,23 @@
         <v>0.0</v>
       </c>
       <c r="N12" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="O12" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="P12" t="n">
         <v>20.0</v>
       </c>
       <c r="Q12" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="R12" t="s">
         <v>8</v>
       </c>
-      <c r="S12"/>
+      <c r="S12" t="s">
+        <v>729</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -8090,14 +8106,14 @@
         <v>548</v>
       </c>
       <c r="E13" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F13" t="n">
         <v>32.0</v>
       </c>
       <c r="G13"/>
       <c r="H13" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I13" t="n">
         <v>1000000.0</v>
@@ -8107,16 +8123,16 @@
       <c r="L13"/>
       <c r="M13"/>
       <c r="N13" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="O13" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="P13" t="n">
         <v>15.0</v>
       </c>
       <c r="Q13" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="R13" t="s">
         <v>9</v>
@@ -8137,7 +8153,7 @@
         <v>549</v>
       </c>
       <c r="E14" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F14" t="n">
         <v>18.0</v>
@@ -8146,7 +8162,7 @@
         <v>10.0</v>
       </c>
       <c r="H14" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I14" t="n">
         <v>351000.0</v>
@@ -8162,22 +8178,22 @@
         <v>37000.0</v>
       </c>
       <c r="N14" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="O14" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="P14" t="n">
         <v>43.0</v>
       </c>
       <c r="Q14" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="R14" t="s">
         <v>511</v>
       </c>
       <c r="S14" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="15">
@@ -8192,7 +8208,7 @@
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F15" t="n">
         <v>9.0</v>
@@ -8201,7 +8217,7 @@
         <v>9.0</v>
       </c>
       <c r="H15" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I15" t="n">
         <v>1190000.0</v>
@@ -8215,22 +8231,22 @@
       </c>
       <c r="M15"/>
       <c r="N15" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="O15" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="P15" t="n">
         <v>8.0</v>
       </c>
       <c r="Q15" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="R15" t="s">
         <v>11</v>
       </c>
       <c r="S15" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="16">
@@ -8254,7 +8270,7 @@
         <v>9.0</v>
       </c>
       <c r="H16" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I16" t="n">
         <v>40000.0</v>
@@ -8268,7 +8284,7 @@
       </c>
       <c r="M16"/>
       <c r="N16" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="O16" t="s">
         <v>95</v>
@@ -8280,10 +8296,10 @@
         <v>95</v>
       </c>
       <c r="R16" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="S16" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="17">
@@ -8300,7 +8316,7 @@
         <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F17" t="n">
         <v>6.0</v>
@@ -8309,7 +8325,7 @@
         <v>6.0</v>
       </c>
       <c r="H17" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I17" t="n">
         <v>32000.0</v>
@@ -8325,22 +8341,22 @@
       </c>
       <c r="M17"/>
       <c r="N17" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="O17" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="P17" t="n">
         <v>6.0</v>
       </c>
       <c r="Q17" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="R17" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="S17" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="18">
@@ -8355,7 +8371,7 @@
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F18" t="n">
         <v>4.0</v>
@@ -8364,7 +8380,7 @@
         <v>4.0</v>
       </c>
       <c r="H18" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I18" t="n">
         <v>22730.0</v>
@@ -8380,7 +8396,7 @@
         <v>1043.0</v>
       </c>
       <c r="N18" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="O18" t="s">
         <v>166</v>
@@ -8392,7 +8408,7 @@
         <v>166</v>
       </c>
       <c r="R18" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="S18" t="s">
         <v>174</v>
@@ -8410,7 +8426,7 @@
       </c>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F19" t="n">
         <v>7.0</v>
@@ -8419,7 +8435,7 @@
         <v>7.0</v>
       </c>
       <c r="H19" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I19" t="n">
         <v>42189.0</v>
@@ -8437,22 +8453,22 @@
         <v>15.0</v>
       </c>
       <c r="N19" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="O19" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="P19" t="n">
         <v>3.0</v>
       </c>
       <c r="Q19" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="R19" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="S19" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="20">
@@ -8467,7 +8483,7 @@
       </c>
       <c r="D20"/>
       <c r="E20" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F20" t="n">
         <v>6.0</v>
@@ -8476,7 +8492,7 @@
         <v>6.0</v>
       </c>
       <c r="H20" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I20" t="n">
         <v>388120.0</v>
@@ -8492,22 +8508,22 @@
         <v>20.0</v>
       </c>
       <c r="N20" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="O20" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="P20" t="n">
         <v>11.0</v>
       </c>
       <c r="Q20" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="R20" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="S20" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="21">
@@ -8524,7 +8540,7 @@
         <v>550</v>
       </c>
       <c r="E21" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F21" t="n">
         <v>18.0</v>
@@ -8533,7 +8549,7 @@
         <v>18.0</v>
       </c>
       <c r="H21" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I21" t="n">
         <v>7960.0</v>
@@ -8545,7 +8561,7 @@
       <c r="L21"/>
       <c r="M21"/>
       <c r="N21" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="O21"/>
       <c r="P21" t="n">
@@ -8555,10 +8571,10 @@
         <v>550</v>
       </c>
       <c r="R21" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="S21" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="22">
@@ -8573,7 +8589,7 @@
       </c>
       <c r="D22"/>
       <c r="E22" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F22" t="n">
         <v>10.0</v>
@@ -8582,7 +8598,7 @@
         <v>6.0</v>
       </c>
       <c r="H22" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I22" t="n">
         <v>5000000.0</v>
@@ -8600,22 +8616,22 @@
         <v>15.0</v>
       </c>
       <c r="N22" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="O22" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="P22" t="n">
         <v>5.0</v>
       </c>
       <c r="Q22" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="R22" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="S22" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="23">
@@ -8630,7 +8646,7 @@
       </c>
       <c r="D23"/>
       <c r="E23" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F23" t="n">
         <v>18.0</v>
@@ -8639,7 +8655,7 @@
         <v>18.0</v>
       </c>
       <c r="H23" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I23" t="n">
         <v>76233.0</v>
@@ -8657,22 +8673,22 @@
         <v>31.0</v>
       </c>
       <c r="N23" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="O23" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="P23" t="n">
         <v>5.0</v>
       </c>
       <c r="Q23" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="R23" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="S23" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="24">
@@ -8687,7 +8703,7 @@
       </c>
       <c r="D24"/>
       <c r="E24" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F24" t="n">
         <v>67.0</v>
@@ -8696,7 +8712,7 @@
         <v>0.0</v>
       </c>
       <c r="H24" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I24"/>
       <c r="J24"/>
@@ -8708,7 +8724,7 @@
       </c>
       <c r="M24"/>
       <c r="N24" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="O24"/>
       <c r="P24" t="n">
@@ -8716,10 +8732,10 @@
       </c>
       <c r="Q24"/>
       <c r="R24" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="S24" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
     </row>
     <row r="25">
@@ -8736,7 +8752,7 @@
         <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F25" t="n">
         <v>43.0</v>
@@ -8745,7 +8761,7 @@
         <v>43.0</v>
       </c>
       <c r="H25" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I25" t="n">
         <v>1000000.0</v>
@@ -8759,7 +8775,7 @@
         <v>100.0</v>
       </c>
       <c r="N25" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="O25"/>
       <c r="P25" t="n">
@@ -8771,7 +8787,9 @@
       <c r="R25" t="s">
         <v>475</v>
       </c>
-      <c r="S25"/>
+      <c r="S25" t="s">
+        <v>739</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -8787,7 +8805,7 @@
         <v>551</v>
       </c>
       <c r="E26" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F26" t="n">
         <v>26.0</v>
@@ -8796,7 +8814,7 @@
         <v>26.0</v>
       </c>
       <c r="H26" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I26" t="n">
         <v>839666.0</v>
@@ -8814,19 +8832,19 @@
         <v>1300.0</v>
       </c>
       <c r="N26" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="O26" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="P26" t="n">
         <v>11.0</v>
       </c>
       <c r="Q26" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="R26" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="S26" t="s">
         <v>740</v>
@@ -8844,7 +8862,7 @@
       </c>
       <c r="D27"/>
       <c r="E27" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F27" t="n">
         <v>18.0</v>
@@ -8853,7 +8871,7 @@
         <v>8.0</v>
       </c>
       <c r="H27" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I27" t="n">
         <v>1941000.0</v>
@@ -8871,22 +8889,22 @@
         <v>270.0</v>
       </c>
       <c r="N27" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="O27" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="P27" t="n">
         <v>9.0</v>
       </c>
       <c r="Q27" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="R27" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="S27" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
     </row>
     <row r="28">
@@ -8901,7 +8919,7 @@
       </c>
       <c r="D28"/>
       <c r="E28" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F28" t="n">
         <v>10.0</v>
@@ -8910,7 +8928,7 @@
         <v>9.0</v>
       </c>
       <c r="H28" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I28" t="n">
         <v>2662777.0</v>
@@ -8926,19 +8944,19 @@
         <v>2560.0</v>
       </c>
       <c r="N28" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="O28" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="P28" t="n">
         <v>9.0</v>
       </c>
       <c r="Q28" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="R28" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="S28" t="s">
         <v>78</v>
@@ -8956,7 +8974,7 @@
       </c>
       <c r="D29"/>
       <c r="E29" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F29" t="n">
         <v>15.0</v>
@@ -8965,7 +8983,7 @@
         <v>0.0</v>
       </c>
       <c r="H29" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I29" t="n">
         <v>190268.0</v>
@@ -8979,7 +8997,7 @@
       <c r="L29"/>
       <c r="M29"/>
       <c r="N29" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="O29" t="s">
         <v>88</v>
@@ -8991,7 +9009,7 @@
         <v>88</v>
       </c>
       <c r="R29" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="S29" t="s">
         <v>741</v>
@@ -9011,14 +9029,14 @@
         <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F30"/>
       <c r="G30" t="n">
         <v>0.0</v>
       </c>
       <c r="H30" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I30"/>
       <c r="J30"/>
@@ -9026,7 +9044,7 @@
       <c r="L30"/>
       <c r="M30"/>
       <c r="N30" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="O30"/>
       <c r="P30" t="n">
@@ -9036,7 +9054,7 @@
         <v>14</v>
       </c>
       <c r="R30" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="S30"/>
     </row>
@@ -9054,7 +9072,7 @@
         <v>552</v>
       </c>
       <c r="E31" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F31" t="n">
         <v>27.0</v>
@@ -9063,7 +9081,7 @@
         <v>27.0</v>
       </c>
       <c r="H31" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I31" t="n">
         <v>89889.0</v>
@@ -9077,19 +9095,19 @@
       </c>
       <c r="M31"/>
       <c r="N31" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="O31" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="P31" t="n">
         <v>12.0</v>
       </c>
       <c r="Q31" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="R31" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="S31" t="s">
         <v>742</v>
@@ -9107,7 +9125,7 @@
       </c>
       <c r="D32"/>
       <c r="E32" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F32" t="n">
         <v>5.0</v>
@@ -9116,7 +9134,7 @@
         <v>3.0</v>
       </c>
       <c r="H32" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I32" t="n">
         <v>315000.0</v>
@@ -9134,7 +9152,7 @@
         <v>52.0</v>
       </c>
       <c r="N32" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="O32" t="s">
         <v>237</v>
@@ -9146,10 +9164,10 @@
         <v>237</v>
       </c>
       <c r="R32" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="S32" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
     </row>
     <row r="33">
@@ -9164,7 +9182,7 @@
       </c>
       <c r="D33"/>
       <c r="E33" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F33" t="n">
         <v>7.0</v>
@@ -9173,7 +9191,7 @@
         <v>7.0</v>
       </c>
       <c r="H33" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I33" t="n">
         <v>83006.0</v>
@@ -9191,7 +9209,7 @@
         <v>28.0</v>
       </c>
       <c r="N33" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="O33" t="s">
         <v>344</v>
@@ -9203,7 +9221,7 @@
         <v>344</v>
       </c>
       <c r="R33" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="S33" t="s">
         <v>743</v>
@@ -9221,14 +9239,14 @@
       </c>
       <c r="D34"/>
       <c r="E34" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F34" t="n">
         <v>6.0</v>
       </c>
       <c r="G34"/>
       <c r="H34" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I34" t="n">
         <v>245000.0</v>
@@ -9238,17 +9256,17 @@
       <c r="L34"/>
       <c r="M34"/>
       <c r="N34" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="O34" t="s">
-        <v>669</v>
+        <v>42</v>
       </c>
       <c r="P34"/>
       <c r="Q34" t="s">
-        <v>669</v>
+        <v>42</v>
       </c>
       <c r="R34" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="S34"/>
     </row>
@@ -9279,14 +9297,14 @@
       <c r="L35"/>
       <c r="M35"/>
       <c r="N35" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="O35" t="s">
-        <v>670</v>
+        <v>199</v>
       </c>
       <c r="P35"/>
       <c r="Q35" t="s">
-        <v>670</v>
+        <v>199</v>
       </c>
       <c r="R35" t="s">
         <v>529</v>
@@ -9322,19 +9340,21 @@
         <v>8.0</v>
       </c>
       <c r="N36" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="O36" t="s">
-        <v>671</v>
+        <v>95</v>
       </c>
       <c r="P36"/>
       <c r="Q36" t="s">
-        <v>671</v>
+        <v>95</v>
       </c>
       <c r="R36" t="s">
-        <v>709</v>
-      </c>
-      <c r="S36"/>
+        <v>706</v>
+      </c>
+      <c r="S36" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
@@ -9347,7 +9367,7 @@
         <v>106</v>
       </c>
       <c r="D37" t="s">
-        <v>553</v>
+        <v>107</v>
       </c>
       <c r="E37" t="s">
         <v>108</v>
@@ -9359,7 +9379,7 @@
         <v>4.0</v>
       </c>
       <c r="H37" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I37"/>
       <c r="J37"/>
@@ -9370,7 +9390,7 @@
       <c r="O37"/>
       <c r="P37"/>
       <c r="Q37" t="s">
-        <v>553</v>
+        <v>107</v>
       </c>
       <c r="R37" t="s">
         <v>106</v>
@@ -9389,7 +9409,7 @@
       </c>
       <c r="D38"/>
       <c r="E38" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F38" t="n">
         <v>4.0</v>
@@ -9404,17 +9424,17 @@
       <c r="L38"/>
       <c r="M38"/>
       <c r="N38" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="O38" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="P38"/>
       <c r="Q38" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="R38" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="S38"/>
     </row>
@@ -9428,7 +9448,7 @@
       </c>
       <c r="D39"/>
       <c r="E39" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F39" t="n">
         <v>29.0</v>
@@ -9437,7 +9457,7 @@
         <v>24.0</v>
       </c>
       <c r="H39" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I39" t="n">
         <v>1221985.0</v>
@@ -9453,20 +9473,20 @@
         <v>600.0</v>
       </c>
       <c r="N39" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="O39" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="P39"/>
       <c r="Q39" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="R39" t="s">
         <v>484</v>
       </c>
       <c r="S39" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="40">
@@ -9481,7 +9501,7 @@
       </c>
       <c r="D40"/>
       <c r="E40" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F40" t="n">
         <v>14.0</v>
@@ -9490,7 +9510,7 @@
         <v>14.0</v>
       </c>
       <c r="H40" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I40"/>
       <c r="J40"/>
@@ -9502,17 +9522,17 @@
         <v>323.0</v>
       </c>
       <c r="N40" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="O40" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="P40"/>
       <c r="Q40" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="R40" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="S40" t="s">
         <v>264</v>
@@ -9530,7 +9550,7 @@
       </c>
       <c r="D41"/>
       <c r="E41" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F41" t="n">
         <v>84.0</v>
@@ -9545,14 +9565,14 @@
       <c r="L41"/>
       <c r="M41"/>
       <c r="N41" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="O41" t="s">
-        <v>675</v>
+        <v>199</v>
       </c>
       <c r="P41"/>
       <c r="Q41" t="s">
-        <v>675</v>
+        <v>199</v>
       </c>
       <c r="R41" t="s">
         <v>533</v>
@@ -9571,7 +9591,7 @@
       </c>
       <c r="D42"/>
       <c r="E42" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F42"/>
       <c r="G42"/>
@@ -9582,17 +9602,17 @@
       <c r="L42"/>
       <c r="M42"/>
       <c r="N42" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="O42" t="s">
-        <v>676</v>
+        <v>208</v>
       </c>
       <c r="P42"/>
       <c r="Q42" t="s">
-        <v>676</v>
+        <v>208</v>
       </c>
       <c r="R42" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="S42"/>
     </row>
@@ -9604,9 +9624,11 @@
       <c r="C43" t="s">
         <v>488</v>
       </c>
-      <c r="D43"/>
+      <c r="D43" t="s">
+        <v>553</v>
+      </c>
       <c r="E43" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F43"/>
       <c r="G43"/>
@@ -9619,19 +9641,19 @@
       <c r="L43"/>
       <c r="M43"/>
       <c r="N43" t="s">
-        <v>646</v>
-      </c>
-      <c r="O43" t="s">
-        <v>677</v>
-      </c>
+        <v>645</v>
+      </c>
+      <c r="O43"/>
       <c r="P43"/>
       <c r="Q43" t="s">
-        <v>677</v>
+        <v>553</v>
       </c>
       <c r="R43" t="s">
         <v>488</v>
       </c>
-      <c r="S43"/>
+      <c r="S43" t="s">
+        <v>746</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
@@ -9647,12 +9669,12 @@
         <v>554</v>
       </c>
       <c r="E44" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F44"/>
       <c r="G44"/>
       <c r="H44" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I44"/>
       <c r="J44"/>
@@ -9666,9 +9688,11 @@
         <v>554</v>
       </c>
       <c r="R44" t="s">
-        <v>713</v>
-      </c>
-      <c r="S44"/>
+        <v>710</v>
+      </c>
+      <c r="S44" t="s">
+        <v>747</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
@@ -9680,12 +9704,12 @@
       </c>
       <c r="D45"/>
       <c r="E45" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F45"/>
       <c r="G45"/>
       <c r="H45" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I45"/>
       <c r="J45"/>
@@ -9693,19 +9717,21 @@
       <c r="L45"/>
       <c r="M45"/>
       <c r="N45" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="O45" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="P45"/>
       <c r="Q45" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="R45" t="s">
         <v>490</v>
       </c>
-      <c r="S45"/>
+      <c r="S45" t="s">
+        <v>748</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
@@ -9726,7 +9752,7 @@
         <v>19.0</v>
       </c>
       <c r="H46" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I46" t="n">
         <v>250000.0</v>
@@ -9746,7 +9772,9 @@
       <c r="R46" t="s">
         <v>252</v>
       </c>
-      <c r="S46"/>
+      <c r="S46" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
@@ -9760,7 +9788,7 @@
       </c>
       <c r="D47"/>
       <c r="E47" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F47" t="n">
         <v>6.0</v>
@@ -9769,7 +9797,7 @@
         <v>6.0</v>
       </c>
       <c r="H47" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I47" t="n">
         <v>136128.0</v>
@@ -9783,14 +9811,14 @@
       <c r="L47"/>
       <c r="M47"/>
       <c r="N47" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="O47" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="P47"/>
       <c r="Q47" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="R47" t="s">
         <v>536</v>
@@ -9813,7 +9841,7 @@
         <v>555</v>
       </c>
       <c r="E48" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F48" t="n">
         <v>20.0</v>
@@ -9826,7 +9854,7 @@
       <c r="L48"/>
       <c r="M48"/>
       <c r="N48" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="O48"/>
       <c r="P48"/>
@@ -9834,7 +9862,7 @@
         <v>555</v>
       </c>
       <c r="R48" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="S48"/>
     </row>
@@ -9849,7 +9877,7 @@
         <v>280</v>
       </c>
       <c r="D49" t="s">
-        <v>556</v>
+        <v>281</v>
       </c>
       <c r="E49" t="s">
         <v>282</v>
@@ -9861,7 +9889,7 @@
         <v>69.0</v>
       </c>
       <c r="H49" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I49" t="n">
         <v>320000.0</v>
@@ -9882,7 +9910,7 @@
       <c r="O49"/>
       <c r="P49"/>
       <c r="Q49" t="s">
-        <v>556</v>
+        <v>281</v>
       </c>
       <c r="R49" t="s">
         <v>280</v>
@@ -9919,14 +9947,14 @@
         <v>295</v>
       </c>
       <c r="O50" t="s">
-        <v>293</v>
+        <v>673</v>
       </c>
       <c r="P50"/>
       <c r="Q50" t="s">
-        <v>293</v>
+        <v>673</v>
       </c>
       <c r="R50" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="S50"/>
     </row>
@@ -9954,11 +9982,11 @@
       <c r="M51"/>
       <c r="N51"/>
       <c r="O51" t="s">
-        <v>336</v>
+        <v>674</v>
       </c>
       <c r="P51"/>
       <c r="Q51" t="s">
-        <v>336</v>
+        <v>674</v>
       </c>
       <c r="R51" t="s">
         <v>335</v>
@@ -9986,7 +10014,7 @@
         <v>13.0</v>
       </c>
       <c r="H52" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I52" t="n">
         <v>44010.0</v>
@@ -10005,17 +10033,17 @@
         <v>342</v>
       </c>
       <c r="O52" t="s">
-        <v>339</v>
+        <v>675</v>
       </c>
       <c r="P52"/>
       <c r="Q52" t="s">
-        <v>339</v>
+        <v>675</v>
       </c>
       <c r="R52" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="S52" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
     </row>
     <row r="53">
@@ -10030,7 +10058,7 @@
       </c>
       <c r="D53"/>
       <c r="E53" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F53" t="n">
         <v>9.0</v>
@@ -10039,7 +10067,7 @@
         <v>9.0</v>
       </c>
       <c r="H53" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I53" t="n">
         <v>50562.0</v>
@@ -10055,20 +10083,20 @@
         <v>450.0</v>
       </c>
       <c r="N53" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="O53" t="s">
-        <v>680</v>
+        <v>350</v>
       </c>
       <c r="P53"/>
       <c r="Q53" t="s">
-        <v>680</v>
+        <v>350</v>
       </c>
       <c r="R53" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="S53" t="s">
-        <v>746</v>
+        <v>750</v>
       </c>
     </row>
     <row r="54">
@@ -10083,7 +10111,7 @@
       </c>
       <c r="D54"/>
       <c r="E54" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F54" t="n">
         <v>6.0</v>
@@ -10099,14 +10127,14 @@
       <c r="M54"/>
       <c r="N54"/>
       <c r="O54" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="P54"/>
       <c r="Q54" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="R54" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="S54"/>
     </row>
@@ -10121,10 +10149,10 @@
         <v>543</v>
       </c>
       <c r="D55" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E55" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F55" t="n">
         <v>10.0</v>
@@ -10133,7 +10161,7 @@
         <v>10.0</v>
       </c>
       <c r="H55" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I55"/>
       <c r="J55"/>
@@ -10146,13 +10174,13 @@
       <c r="O55"/>
       <c r="P55"/>
       <c r="Q55" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="R55" t="s">
         <v>543</v>
       </c>
       <c r="S55" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
     </row>
     <row r="56">
@@ -10181,14 +10209,14 @@
         <v>423</v>
       </c>
       <c r="O56" t="s">
-        <v>421</v>
+        <v>677</v>
       </c>
       <c r="P56"/>
       <c r="Q56" t="s">
-        <v>421</v>
+        <v>677</v>
       </c>
       <c r="R56" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="S56"/>
     </row>
@@ -10204,7 +10232,7 @@
       </c>
       <c r="D57"/>
       <c r="E57" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F57"/>
       <c r="G57"/>
@@ -10216,14 +10244,14 @@
       <c r="M57"/>
       <c r="N57"/>
       <c r="O57" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="P57"/>
       <c r="Q57" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="R57" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="S57"/>
     </row>
@@ -10254,7 +10282,7 @@
       <c r="P58"/>
       <c r="Q58"/>
       <c r="R58" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="S58"/>
     </row>
@@ -10286,14 +10314,14 @@
         <v>441</v>
       </c>
       <c r="O59" t="s">
-        <v>438</v>
+        <v>679</v>
       </c>
       <c r="P59"/>
       <c r="Q59" t="s">
-        <v>438</v>
+        <v>679</v>
       </c>
       <c r="R59" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="S59"/>
     </row>

</xml_diff>

<commit_message>
Country names in the output of Table 1 change to country codes
</commit_message>
<xml_diff>
--- a/dat/synchros-initiatives.xlsx
+++ b/dat/synchros-initiatives.xlsx
@@ -13,8 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="3" r:id="rId1"/>
-    <sheet name="Table 1 updated" r:id="rId7" sheetId="6"/>
-    <sheet name="Table 1 complete" r:id="rId6" sheetId="7"/>
+    <sheet name="Table 1 updated" r:id="rId7" sheetId="12"/>
+    <sheet name="Table 1 complete" r:id="rId6" sheetId="13"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4829" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10539" uniqueCount="892">
   <si>
     <t>A consortium of agricultural cohort studies</t>
   </si>
@@ -2632,6 +2632,132 @@
   </si>
   <si>
     <t>Mix</t>
+  </si>
+  <si>
+    <t>AUS, CAN, CHL, CRI, DNK, FRA, NZL, NOR, KOR, ZAF, GBR, USA</t>
+  </si>
+  <si>
+    <t>CUB, MEX, DOM, PRI, CHN, PER, IND, VEN, AUT, AUS, GRC, ESP, FIN, POL, GBR, RUS, LTU, CZE, USA, JPN, GHA, NLD, KOR, ZAF, DNK, HUN, SWE, CHE, IRL, EST, BEL, ISR, SVN, HRV, LUX, PRT, FRA, DEU, ITA</t>
+  </si>
+  <si>
+    <t>NLD</t>
+  </si>
+  <si>
+    <t>CAN, DEU, ITA, IRL, GBR, FIN, NLD, NOR</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>SWE</t>
+  </si>
+  <si>
+    <t>ESP</t>
+  </si>
+  <si>
+    <t>GBR, FIN</t>
+  </si>
+  <si>
+    <t>NLD, ESP, GBR, DNK, SWE, BEL, NOR, FRA, FIN, GRC, DEU, CYP</t>
+  </si>
+  <si>
+    <t>DEU, ITA, NLD, ESP, GBR, SWE</t>
+  </si>
+  <si>
+    <t>CAN, NOR, FRA, DNK, EST, DEU, GRC, ITA, LTU, POL, RUS, IRL, PRT, BEL, ESP, SWE, NLD, GBR, FIN, AUS</t>
+  </si>
+  <si>
+    <t>DEU, GBR, FIN, EST, DNK, ITA, ESP, LTU, AUS, SWE, RUS, POL, FRA, NOR, CAN</t>
+  </si>
+  <si>
+    <t>USA, MEX, ISR, CRI, KOR, JPN, CHN, IND, GBR, AUT, BEL, HRV, CYP, CZE, DNK, EST, FIN, FRA, DEU, GRC, HUN, ITA, LVA, LTU, LUX, MLT, NLD, POL, PRT, ROU, SVK, SVN, ESP, SWE, CHE, IRL, IDN, GHA, RUS, ZAF, BRA, THA, MYS</t>
+  </si>
+  <si>
+    <t>DNK, FIN, ITA, NLD, NOR, GBR, AUS, SWE</t>
+  </si>
+  <si>
+    <t>GBR</t>
+  </si>
+  <si>
+    <t>FRA, GRC, LTU, NOR, ESP, GBR</t>
+  </si>
+  <si>
+    <t>CAN, CHN, IND, ZAF</t>
+  </si>
+  <si>
+    <t>USA, FIN, AUS</t>
+  </si>
+  <si>
+    <t>AUS, DNK, BRA, CHN, FRA, ITA, ISR, JPN, NOR, GBR, USA</t>
+  </si>
+  <si>
+    <t>SWE, GBR, FIN, FRA, DNK</t>
+  </si>
+  <si>
+    <t>SWE, DNK, FIN, USA, AUS</t>
+  </si>
+  <si>
+    <t>AUS, GBR, DNK, FRA, JPN, USA, LBN, ESP, SWE, MAR, CHN</t>
+  </si>
+  <si>
+    <t>GBR, IRL, PRT, FRA, CHE, ITA, FIN, USA, AUS</t>
+  </si>
+  <si>
+    <t>CAN, NLD, RUS, POL, NOR, DEU, USA, FRA, ITA</t>
+  </si>
+  <si>
+    <t>ARG, AUS, BEL, BRA, CAN, CHL, HRV, EGY, EST, DEU, GRC, HUN</t>
+  </si>
+  <si>
+    <t>ZAF</t>
+  </si>
+  <si>
+    <t>DNK</t>
+  </si>
+  <si>
+    <t>KOR, VNM, KHM, JPN, CHN</t>
+  </si>
+  <si>
+    <t>CAN, CHN</t>
+  </si>
+  <si>
+    <t>BGD, JPN, TWN, KOR, CHN, IND, SGP, IRN, MNG, SGP, MYS, USA</t>
+  </si>
+  <si>
+    <t>GBR, NLD, DEU, FRA, DNK, GRC, FIN, NOR, SWE, USA</t>
+  </si>
+  <si>
+    <t>FIN</t>
+  </si>
+  <si>
+    <t>JPN</t>
+  </si>
+  <si>
+    <t>CHN, GHA, IND, MEX, RUS, ZAF, GBR, USA, AUT, BEL, DNK, FRA, DEU, GRC, ITA, CHE, NLD, ESP, SWE</t>
+  </si>
+  <si>
+    <t>BEL, CZE, DNK, FRO, FIN, FRA, DEU, GRC, IRL, ITA, LTU, NLD, NOR, POL, PRT, SVK, ESP, SWE, CHE, UKR, GBR</t>
+  </si>
+  <si>
+    <t>NOR, FIN, SWE, GBR, NLD, FRA, ESP, ITA</t>
+  </si>
+  <si>
+    <t>ESP, SWE, GBR, DNK, NOR, FRA, DEU, NLD, GRC, ITA</t>
+  </si>
+  <si>
+    <t>AUS</t>
+  </si>
+  <si>
+    <t>USA, SWE, FIN</t>
+  </si>
+  <si>
+    <t>ITA, NLD, GBR, SWE</t>
+  </si>
+  <si>
+    <t>CAN, FRA</t>
+  </si>
+  <si>
+    <t>FIN, DNK, NLD, DEU, ESP, BEL, ITA, POL</t>
   </si>
 </sst>
 </file>
@@ -7713,7 +7839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -7826,13 +7952,13 @@
         <v>651</v>
       </c>
       <c r="P2" t="s">
-        <v>673</v>
+        <v>850</v>
       </c>
       <c r="Q2" t="n">
         <v>12.0</v>
       </c>
       <c r="R2" t="s">
-        <v>673</v>
+        <v>850</v>
       </c>
       <c r="S2" t="s">
         <v>703</v>
@@ -7886,13 +8012,13 @@
         <v>652</v>
       </c>
       <c r="P3" t="s">
-        <v>674</v>
+        <v>851</v>
       </c>
       <c r="Q3" t="n">
         <v>39.0</v>
       </c>
       <c r="R3" t="s">
-        <v>674</v>
+        <v>851</v>
       </c>
       <c r="S3" t="s">
         <v>704</v>
@@ -7944,13 +8070,13 @@
         <v>653</v>
       </c>
       <c r="P4" t="s">
-        <v>183</v>
+        <v>852</v>
       </c>
       <c r="Q4" t="n">
         <v>1.0</v>
       </c>
       <c r="R4" t="s">
-        <v>183</v>
+        <v>852</v>
       </c>
       <c r="S4" t="s">
         <v>5</v>
@@ -8000,13 +8126,13 @@
         <v>654</v>
       </c>
       <c r="P5" t="s">
-        <v>71</v>
+        <v>853</v>
       </c>
       <c r="Q5" t="n">
         <v>8.0</v>
       </c>
       <c r="R5" t="s">
-        <v>71</v>
+        <v>853</v>
       </c>
       <c r="S5" t="s">
         <v>705</v>
@@ -8060,13 +8186,13 @@
         <v>655</v>
       </c>
       <c r="P6" t="s">
-        <v>60</v>
+        <v>854</v>
       </c>
       <c r="Q6" t="n">
         <v>1.0</v>
       </c>
       <c r="R6" t="s">
-        <v>60</v>
+        <v>854</v>
       </c>
       <c r="S6" t="s">
         <v>706</v>
@@ -8120,13 +8246,13 @@
         <v>656</v>
       </c>
       <c r="P7" t="s">
-        <v>88</v>
+        <v>855</v>
       </c>
       <c r="Q7" t="n">
         <v>1.0</v>
       </c>
       <c r="R7" t="s">
-        <v>88</v>
+        <v>855</v>
       </c>
       <c r="S7" t="s">
         <v>707</v>
@@ -8180,13 +8306,13 @@
         <v>657</v>
       </c>
       <c r="P8" t="s">
-        <v>304</v>
+        <v>856</v>
       </c>
       <c r="Q8" t="n">
         <v>1.0</v>
       </c>
       <c r="R8" t="s">
-        <v>304</v>
+        <v>856</v>
       </c>
       <c r="S8" t="s">
         <v>708</v>
@@ -8240,13 +8366,13 @@
         <v>658</v>
       </c>
       <c r="P9" t="s">
-        <v>675</v>
+        <v>857</v>
       </c>
       <c r="Q9" t="n">
         <v>2.0</v>
       </c>
       <c r="R9" t="s">
-        <v>675</v>
+        <v>857</v>
       </c>
       <c r="S9" t="s">
         <v>709</v>
@@ -8294,13 +8420,13 @@
       </c>
       <c r="O10"/>
       <c r="P10" t="s">
-        <v>676</v>
+        <v>858</v>
       </c>
       <c r="Q10" t="n">
         <v>12.0</v>
       </c>
       <c r="R10" t="s">
-        <v>676</v>
+        <v>858</v>
       </c>
       <c r="S10" t="s">
         <v>710</v>
@@ -8354,13 +8480,13 @@
         <v>659</v>
       </c>
       <c r="P11" t="s">
-        <v>677</v>
+        <v>859</v>
       </c>
       <c r="Q11" t="n">
         <v>6.0</v>
       </c>
       <c r="R11" t="s">
-        <v>677</v>
+        <v>859</v>
       </c>
       <c r="S11" t="s">
         <v>409</v>
@@ -8404,13 +8530,13 @@
       </c>
       <c r="O12"/>
       <c r="P12" t="s">
-        <v>678</v>
+        <v>860</v>
       </c>
       <c r="Q12" t="n">
         <v>20.0</v>
       </c>
       <c r="R12" t="s">
-        <v>678</v>
+        <v>860</v>
       </c>
       <c r="S12" t="s">
         <v>8</v>
@@ -8456,13 +8582,13 @@
         <v>660</v>
       </c>
       <c r="P13" t="s">
-        <v>679</v>
+        <v>861</v>
       </c>
       <c r="Q13" t="n">
         <v>15.0</v>
       </c>
       <c r="R13" t="s">
-        <v>679</v>
+        <v>861</v>
       </c>
       <c r="S13" t="s">
         <v>9</v>
@@ -8514,13 +8640,13 @@
         <v>661</v>
       </c>
       <c r="P14" t="s">
-        <v>680</v>
+        <v>862</v>
       </c>
       <c r="Q14" t="n">
         <v>43.0</v>
       </c>
       <c r="R14" t="s">
-        <v>680</v>
+        <v>862</v>
       </c>
       <c r="S14" t="s">
         <v>512</v>
@@ -8570,13 +8696,13 @@
         <v>662</v>
       </c>
       <c r="P15" t="s">
-        <v>681</v>
+        <v>863</v>
       </c>
       <c r="Q15" t="n">
         <v>8.0</v>
       </c>
       <c r="R15" t="s">
-        <v>681</v>
+        <v>863</v>
       </c>
       <c r="S15" t="s">
         <v>11</v>
@@ -8626,13 +8752,13 @@
         <v>661</v>
       </c>
       <c r="P16" t="s">
-        <v>95</v>
+        <v>864</v>
       </c>
       <c r="Q16" t="n">
         <v>1.0</v>
       </c>
       <c r="R16" t="s">
-        <v>95</v>
+        <v>864</v>
       </c>
       <c r="S16" t="s">
         <v>711</v>
@@ -8686,13 +8812,13 @@
         <v>663</v>
       </c>
       <c r="P17" t="s">
-        <v>682</v>
+        <v>865</v>
       </c>
       <c r="Q17" t="n">
         <v>6.0</v>
       </c>
       <c r="R17" t="s">
-        <v>682</v>
+        <v>865</v>
       </c>
       <c r="S17" t="s">
         <v>712</v>
@@ -8744,13 +8870,13 @@
         <v>664</v>
       </c>
       <c r="P18" t="s">
-        <v>166</v>
+        <v>866</v>
       </c>
       <c r="Q18" t="n">
         <v>4.0</v>
       </c>
       <c r="R18" t="s">
-        <v>166</v>
+        <v>866</v>
       </c>
       <c r="S18" t="s">
         <v>713</v>
@@ -8804,13 +8930,13 @@
         <v>660</v>
       </c>
       <c r="P19" t="s">
-        <v>683</v>
+        <v>867</v>
       </c>
       <c r="Q19" t="n">
         <v>3.0</v>
       </c>
       <c r="R19" t="s">
-        <v>683</v>
+        <v>867</v>
       </c>
       <c r="S19" t="s">
         <v>714</v>
@@ -8862,13 +8988,13 @@
         <v>665</v>
       </c>
       <c r="P20" t="s">
-        <v>684</v>
+        <v>868</v>
       </c>
       <c r="Q20" t="n">
         <v>11.0</v>
       </c>
       <c r="R20" t="s">
-        <v>684</v>
+        <v>868</v>
       </c>
       <c r="S20" t="s">
         <v>715</v>
@@ -8974,13 +9100,13 @@
       </c>
       <c r="O22"/>
       <c r="P22" t="s">
-        <v>685</v>
+        <v>869</v>
       </c>
       <c r="Q22" t="n">
         <v>5.0</v>
       </c>
       <c r="R22" t="s">
-        <v>685</v>
+        <v>869</v>
       </c>
       <c r="S22" t="s">
         <v>717</v>
@@ -9032,13 +9158,13 @@
       </c>
       <c r="O23"/>
       <c r="P23" t="s">
-        <v>686</v>
+        <v>870</v>
       </c>
       <c r="Q23" t="n">
         <v>5.0</v>
       </c>
       <c r="R23" t="s">
-        <v>686</v>
+        <v>870</v>
       </c>
       <c r="S23" t="s">
         <v>718</v>
@@ -9200,13 +9326,13 @@
         <v>668</v>
       </c>
       <c r="P26" t="s">
-        <v>687</v>
+        <v>871</v>
       </c>
       <c r="Q26" t="n">
         <v>11.0</v>
       </c>
       <c r="R26" t="s">
-        <v>687</v>
+        <v>871</v>
       </c>
       <c r="S26" t="s">
         <v>720</v>
@@ -9260,13 +9386,13 @@
         <v>669</v>
       </c>
       <c r="P27" t="s">
-        <v>688</v>
+        <v>872</v>
       </c>
       <c r="Q27" t="n">
         <v>9.0</v>
       </c>
       <c r="R27" t="s">
-        <v>688</v>
+        <v>872</v>
       </c>
       <c r="S27" t="s">
         <v>721</v>
@@ -9318,13 +9444,13 @@
         <v>670</v>
       </c>
       <c r="P28" t="s">
-        <v>689</v>
+        <v>873</v>
       </c>
       <c r="Q28" t="n">
         <v>9.0</v>
       </c>
       <c r="R28" t="s">
-        <v>689</v>
+        <v>873</v>
       </c>
       <c r="S28" t="s">
         <v>722</v>
@@ -9372,13 +9498,13 @@
       </c>
       <c r="O29"/>
       <c r="P29" t="s">
-        <v>88</v>
+        <v>855</v>
       </c>
       <c r="Q29" t="n">
         <v>1.0</v>
       </c>
       <c r="R29" t="s">
-        <v>88</v>
+        <v>855</v>
       </c>
       <c r="S29" t="s">
         <v>723</v>
@@ -9474,13 +9600,13 @@
         <v>664</v>
       </c>
       <c r="P31" t="s">
-        <v>690</v>
+        <v>874</v>
       </c>
       <c r="Q31" t="n">
         <v>12.0</v>
       </c>
       <c r="R31" t="s">
-        <v>690</v>
+        <v>874</v>
       </c>
       <c r="S31" t="s">
         <v>725</v>
@@ -9534,13 +9660,13 @@
         <v>671</v>
       </c>
       <c r="P32" t="s">
-        <v>237</v>
+        <v>875</v>
       </c>
       <c r="Q32" t="n">
         <v>1.0</v>
       </c>
       <c r="R32" t="s">
-        <v>237</v>
+        <v>875</v>
       </c>
       <c r="S32" t="s">
         <v>726</v>
@@ -9594,13 +9720,13 @@
         <v>672</v>
       </c>
       <c r="P33" t="s">
-        <v>344</v>
+        <v>876</v>
       </c>
       <c r="Q33" t="n">
         <v>1.0</v>
       </c>
       <c r="R33" t="s">
-        <v>344</v>
+        <v>876</v>
       </c>
       <c r="S33" t="s">
         <v>727</v>
@@ -9642,11 +9768,11 @@
       </c>
       <c r="O34"/>
       <c r="P34" t="s">
-        <v>42</v>
+        <v>877</v>
       </c>
       <c r="Q34"/>
       <c r="R34" t="s">
-        <v>42</v>
+        <v>877</v>
       </c>
       <c r="S34" t="s">
         <v>728</v>
@@ -9684,11 +9810,11 @@
       </c>
       <c r="O35"/>
       <c r="P35" t="s">
-        <v>199</v>
+        <v>839</v>
       </c>
       <c r="Q35"/>
       <c r="R35" t="s">
-        <v>199</v>
+        <v>839</v>
       </c>
       <c r="S35" t="s">
         <v>530</v>
@@ -9728,11 +9854,11 @@
       </c>
       <c r="O36"/>
       <c r="P36" t="s">
-        <v>95</v>
+        <v>864</v>
       </c>
       <c r="Q36"/>
       <c r="R36" t="s">
-        <v>95</v>
+        <v>864</v>
       </c>
       <c r="S36" t="s">
         <v>729</v>
@@ -9814,11 +9940,11 @@
       </c>
       <c r="O38"/>
       <c r="P38" t="s">
-        <v>691</v>
+        <v>878</v>
       </c>
       <c r="Q38"/>
       <c r="R38" t="s">
-        <v>691</v>
+        <v>878</v>
       </c>
       <c r="S38" t="s">
         <v>730</v>
@@ -9864,11 +9990,11 @@
       </c>
       <c r="O39"/>
       <c r="P39" t="s">
-        <v>692</v>
+        <v>879</v>
       </c>
       <c r="Q39"/>
       <c r="R39" t="s">
-        <v>692</v>
+        <v>879</v>
       </c>
       <c r="S39" t="s">
         <v>485</v>
@@ -9914,11 +10040,11 @@
       </c>
       <c r="O40"/>
       <c r="P40" t="s">
-        <v>693</v>
+        <v>880</v>
       </c>
       <c r="Q40"/>
       <c r="R40" t="s">
-        <v>693</v>
+        <v>880</v>
       </c>
       <c r="S40" t="s">
         <v>731</v>
@@ -9958,11 +10084,11 @@
       </c>
       <c r="O41"/>
       <c r="P41" t="s">
-        <v>199</v>
+        <v>839</v>
       </c>
       <c r="Q41"/>
       <c r="R41" t="s">
-        <v>199</v>
+        <v>839</v>
       </c>
       <c r="S41" t="s">
         <v>534</v>
@@ -9996,11 +10122,11 @@
       </c>
       <c r="O42"/>
       <c r="P42" t="s">
-        <v>208</v>
+        <v>881</v>
       </c>
       <c r="Q42"/>
       <c r="R42" t="s">
-        <v>208</v>
+        <v>881</v>
       </c>
       <c r="S42" t="s">
         <v>732</v>
@@ -10114,11 +10240,11 @@
       </c>
       <c r="O45"/>
       <c r="P45" t="s">
-        <v>694</v>
+        <v>882</v>
       </c>
       <c r="Q45"/>
       <c r="R45" t="s">
-        <v>694</v>
+        <v>882</v>
       </c>
       <c r="S45" t="s">
         <v>491</v>
@@ -10210,11 +10336,11 @@
       </c>
       <c r="O47"/>
       <c r="P47" t="s">
-        <v>695</v>
+        <v>883</v>
       </c>
       <c r="Q47"/>
       <c r="R47" t="s">
-        <v>695</v>
+        <v>883</v>
       </c>
       <c r="S47" t="s">
         <v>537</v>
@@ -10346,11 +10472,11 @@
       </c>
       <c r="O50"/>
       <c r="P50" t="s">
-        <v>696</v>
+        <v>884</v>
       </c>
       <c r="Q50"/>
       <c r="R50" t="s">
-        <v>696</v>
+        <v>884</v>
       </c>
       <c r="S50" t="s">
         <v>735</v>
@@ -10382,11 +10508,11 @@
       <c r="N51"/>
       <c r="O51"/>
       <c r="P51" t="s">
-        <v>697</v>
+        <v>885</v>
       </c>
       <c r="Q51"/>
       <c r="R51" t="s">
-        <v>697</v>
+        <v>885</v>
       </c>
       <c r="S51" t="s">
         <v>335</v>
@@ -10434,11 +10560,11 @@
       </c>
       <c r="O52"/>
       <c r="P52" t="s">
-        <v>698</v>
+        <v>886</v>
       </c>
       <c r="Q52"/>
       <c r="R52" t="s">
-        <v>698</v>
+        <v>886</v>
       </c>
       <c r="S52" t="s">
         <v>736</v>
@@ -10488,11 +10614,11 @@
       </c>
       <c r="O53"/>
       <c r="P53" t="s">
-        <v>350</v>
+        <v>887</v>
       </c>
       <c r="Q53"/>
       <c r="R53" t="s">
-        <v>350</v>
+        <v>887</v>
       </c>
       <c r="S53" t="s">
         <v>737</v>
@@ -10530,11 +10656,11 @@
       <c r="N54"/>
       <c r="O54"/>
       <c r="P54" t="s">
-        <v>699</v>
+        <v>888</v>
       </c>
       <c r="Q54"/>
       <c r="R54" t="s">
-        <v>699</v>
+        <v>888</v>
       </c>
       <c r="S54" t="s">
         <v>738</v>
@@ -10614,11 +10740,11 @@
       </c>
       <c r="O56"/>
       <c r="P56" t="s">
-        <v>700</v>
+        <v>889</v>
       </c>
       <c r="Q56"/>
       <c r="R56" t="s">
-        <v>700</v>
+        <v>889</v>
       </c>
       <c r="S56" t="s">
         <v>739</v>
@@ -10650,11 +10776,11 @@
       <c r="N57"/>
       <c r="O57"/>
       <c r="P57" t="s">
-        <v>701</v>
+        <v>890</v>
       </c>
       <c r="Q57"/>
       <c r="R57" t="s">
-        <v>701</v>
+        <v>890</v>
       </c>
       <c r="S57" t="s">
         <v>740</v>
@@ -10722,11 +10848,11 @@
       </c>
       <c r="O59"/>
       <c r="P59" t="s">
-        <v>702</v>
+        <v>891</v>
       </c>
       <c r="Q59"/>
       <c r="R59" t="s">
-        <v>702</v>
+        <v>891</v>
       </c>
       <c r="S59" t="s">
         <v>742</v>
@@ -10738,7 +10864,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -10887,13 +11013,13 @@
         <v>651</v>
       </c>
       <c r="P2" t="s">
-        <v>673</v>
+        <v>850</v>
       </c>
       <c r="Q2" t="n">
         <v>12.0</v>
       </c>
       <c r="R2" t="s">
-        <v>673</v>
+        <v>850</v>
       </c>
       <c r="S2" t="s">
         <v>703</v>
@@ -10975,13 +11101,13 @@
         <v>652</v>
       </c>
       <c r="P3" t="s">
-        <v>674</v>
+        <v>851</v>
       </c>
       <c r="Q3" t="n">
         <v>39.0</v>
       </c>
       <c r="R3" t="s">
-        <v>674</v>
+        <v>851</v>
       </c>
       <c r="S3" t="s">
         <v>704</v>
@@ -11063,13 +11189,13 @@
         <v>653</v>
       </c>
       <c r="P4" t="s">
-        <v>183</v>
+        <v>852</v>
       </c>
       <c r="Q4" t="n">
         <v>1.0</v>
       </c>
       <c r="R4" t="s">
-        <v>183</v>
+        <v>852</v>
       </c>
       <c r="S4" t="s">
         <v>5</v>
@@ -11141,13 +11267,13 @@
         <v>654</v>
       </c>
       <c r="P5" t="s">
-        <v>71</v>
+        <v>853</v>
       </c>
       <c r="Q5" t="n">
         <v>8.0</v>
       </c>
       <c r="R5" t="s">
-        <v>71</v>
+        <v>853</v>
       </c>
       <c r="S5" t="s">
         <v>705</v>
@@ -11233,13 +11359,13 @@
         <v>655</v>
       </c>
       <c r="P6" t="s">
-        <v>60</v>
+        <v>854</v>
       </c>
       <c r="Q6" t="n">
         <v>1.0</v>
       </c>
       <c r="R6" t="s">
-        <v>60</v>
+        <v>854</v>
       </c>
       <c r="S6" t="s">
         <v>706</v>
@@ -11325,13 +11451,13 @@
         <v>656</v>
       </c>
       <c r="P7" t="s">
-        <v>88</v>
+        <v>855</v>
       </c>
       <c r="Q7" t="n">
         <v>1.0</v>
       </c>
       <c r="R7" t="s">
-        <v>88</v>
+        <v>855</v>
       </c>
       <c r="S7" t="s">
         <v>707</v>
@@ -11411,13 +11537,13 @@
         <v>657</v>
       </c>
       <c r="P8" t="s">
-        <v>304</v>
+        <v>856</v>
       </c>
       <c r="Q8" t="n">
         <v>1.0</v>
       </c>
       <c r="R8" t="s">
-        <v>304</v>
+        <v>856</v>
       </c>
       <c r="S8" t="s">
         <v>708</v>
@@ -11503,13 +11629,13 @@
         <v>658</v>
       </c>
       <c r="P9" t="s">
-        <v>675</v>
+        <v>857</v>
       </c>
       <c r="Q9" t="n">
         <v>2.0</v>
       </c>
       <c r="R9" t="s">
-        <v>675</v>
+        <v>857</v>
       </c>
       <c r="S9" t="s">
         <v>709</v>
@@ -11581,13 +11707,13 @@
       </c>
       <c r="O10"/>
       <c r="P10" t="s">
-        <v>676</v>
+        <v>858</v>
       </c>
       <c r="Q10" t="n">
         <v>12.0</v>
       </c>
       <c r="R10" t="s">
-        <v>676</v>
+        <v>858</v>
       </c>
       <c r="S10" t="s">
         <v>710</v>
@@ -11665,13 +11791,13 @@
         <v>659</v>
       </c>
       <c r="P11" t="s">
-        <v>677</v>
+        <v>859</v>
       </c>
       <c r="Q11" t="n">
         <v>6.0</v>
       </c>
       <c r="R11" t="s">
-        <v>677</v>
+        <v>859</v>
       </c>
       <c r="S11" t="s">
         <v>409</v>
@@ -11741,13 +11867,13 @@
       </c>
       <c r="O12"/>
       <c r="P12" t="s">
-        <v>678</v>
+        <v>860</v>
       </c>
       <c r="Q12" t="n">
         <v>20.0</v>
       </c>
       <c r="R12" t="s">
-        <v>678</v>
+        <v>860</v>
       </c>
       <c r="S12" t="s">
         <v>8</v>
@@ -11817,13 +11943,13 @@
         <v>660</v>
       </c>
       <c r="P13" t="s">
-        <v>679</v>
+        <v>861</v>
       </c>
       <c r="Q13" t="n">
         <v>15.0</v>
       </c>
       <c r="R13" t="s">
-        <v>679</v>
+        <v>861</v>
       </c>
       <c r="S13" t="s">
         <v>9</v>
@@ -11903,13 +12029,13 @@
         <v>661</v>
       </c>
       <c r="P14" t="s">
-        <v>680</v>
+        <v>862</v>
       </c>
       <c r="Q14" t="n">
         <v>43.0</v>
       </c>
       <c r="R14" t="s">
-        <v>680</v>
+        <v>862</v>
       </c>
       <c r="S14" t="s">
         <v>512</v>
@@ -11991,13 +12117,13 @@
         <v>662</v>
       </c>
       <c r="P15" t="s">
-        <v>681</v>
+        <v>863</v>
       </c>
       <c r="Q15" t="n">
         <v>8.0</v>
       </c>
       <c r="R15" t="s">
-        <v>681</v>
+        <v>863</v>
       </c>
       <c r="S15" t="s">
         <v>11</v>
@@ -12071,13 +12197,13 @@
         <v>661</v>
       </c>
       <c r="P16" t="s">
-        <v>95</v>
+        <v>864</v>
       </c>
       <c r="Q16" t="n">
         <v>1.0</v>
       </c>
       <c r="R16" t="s">
-        <v>95</v>
+        <v>864</v>
       </c>
       <c r="S16" t="s">
         <v>711</v>
@@ -12157,13 +12283,13 @@
         <v>663</v>
       </c>
       <c r="P17" t="s">
-        <v>682</v>
+        <v>865</v>
       </c>
       <c r="Q17" t="n">
         <v>6.0</v>
       </c>
       <c r="R17" t="s">
-        <v>682</v>
+        <v>865</v>
       </c>
       <c r="S17" t="s">
         <v>712</v>
@@ -12247,13 +12373,13 @@
         <v>664</v>
       </c>
       <c r="P18" t="s">
-        <v>166</v>
+        <v>866</v>
       </c>
       <c r="Q18" t="n">
         <v>4.0</v>
       </c>
       <c r="R18" t="s">
-        <v>166</v>
+        <v>866</v>
       </c>
       <c r="S18" t="s">
         <v>713</v>
@@ -12329,13 +12455,13 @@
         <v>660</v>
       </c>
       <c r="P19" t="s">
-        <v>683</v>
+        <v>867</v>
       </c>
       <c r="Q19" t="n">
         <v>3.0</v>
       </c>
       <c r="R19" t="s">
-        <v>683</v>
+        <v>867</v>
       </c>
       <c r="S19" t="s">
         <v>714</v>
@@ -12413,13 +12539,13 @@
         <v>665</v>
       </c>
       <c r="P20" t="s">
-        <v>684</v>
+        <v>868</v>
       </c>
       <c r="Q20" t="n">
         <v>11.0</v>
       </c>
       <c r="R20" t="s">
-        <v>684</v>
+        <v>868</v>
       </c>
       <c r="S20" t="s">
         <v>715</v>
@@ -12563,13 +12689,13 @@
       </c>
       <c r="O22"/>
       <c r="P22" t="s">
-        <v>685</v>
+        <v>869</v>
       </c>
       <c r="Q22" t="n">
         <v>5.0</v>
       </c>
       <c r="R22" t="s">
-        <v>685</v>
+        <v>869</v>
       </c>
       <c r="S22" t="s">
         <v>717</v>
@@ -12643,13 +12769,13 @@
       </c>
       <c r="O23"/>
       <c r="P23" t="s">
-        <v>686</v>
+        <v>870</v>
       </c>
       <c r="Q23" t="n">
         <v>5.0</v>
       </c>
       <c r="R23" t="s">
-        <v>686</v>
+        <v>870</v>
       </c>
       <c r="S23" t="s">
         <v>718</v>
@@ -12891,13 +13017,13 @@
         <v>668</v>
       </c>
       <c r="P26" t="s">
-        <v>687</v>
+        <v>871</v>
       </c>
       <c r="Q26" t="n">
         <v>11.0</v>
       </c>
       <c r="R26" t="s">
-        <v>687</v>
+        <v>871</v>
       </c>
       <c r="S26" t="s">
         <v>720</v>
@@ -12975,13 +13101,13 @@
         <v>669</v>
       </c>
       <c r="P27" t="s">
-        <v>688</v>
+        <v>872</v>
       </c>
       <c r="Q27" t="n">
         <v>9.0</v>
       </c>
       <c r="R27" t="s">
-        <v>688</v>
+        <v>872</v>
       </c>
       <c r="S27" t="s">
         <v>721</v>
@@ -13059,13 +13185,13 @@
         <v>670</v>
       </c>
       <c r="P28" t="s">
-        <v>689</v>
+        <v>873</v>
       </c>
       <c r="Q28" t="n">
         <v>9.0</v>
       </c>
       <c r="R28" t="s">
-        <v>689</v>
+        <v>873</v>
       </c>
       <c r="S28" t="s">
         <v>722</v>
@@ -13143,13 +13269,13 @@
       </c>
       <c r="O29"/>
       <c r="P29" t="s">
-        <v>88</v>
+        <v>855</v>
       </c>
       <c r="Q29" t="n">
         <v>1.0</v>
       </c>
       <c r="R29" t="s">
-        <v>88</v>
+        <v>855</v>
       </c>
       <c r="S29" t="s">
         <v>723</v>
@@ -13305,13 +13431,13 @@
         <v>664</v>
       </c>
       <c r="P31" t="s">
-        <v>690</v>
+        <v>874</v>
       </c>
       <c r="Q31" t="n">
         <v>12.0</v>
       </c>
       <c r="R31" t="s">
-        <v>690</v>
+        <v>874</v>
       </c>
       <c r="S31" t="s">
         <v>725</v>
@@ -13393,13 +13519,13 @@
         <v>671</v>
       </c>
       <c r="P32" t="s">
-        <v>237</v>
+        <v>875</v>
       </c>
       <c r="Q32" t="n">
         <v>1.0</v>
       </c>
       <c r="R32" t="s">
-        <v>237</v>
+        <v>875</v>
       </c>
       <c r="S32" t="s">
         <v>726</v>
@@ -13481,13 +13607,13 @@
         <v>672</v>
       </c>
       <c r="P33" t="s">
-        <v>344</v>
+        <v>876</v>
       </c>
       <c r="Q33" t="n">
         <v>1.0</v>
       </c>
       <c r="R33" t="s">
-        <v>344</v>
+        <v>876</v>
       </c>
       <c r="S33" t="s">
         <v>727</v>
@@ -13555,11 +13681,11 @@
       </c>
       <c r="O34"/>
       <c r="P34" t="s">
-        <v>42</v>
+        <v>877</v>
       </c>
       <c r="Q34"/>
       <c r="R34" t="s">
-        <v>42</v>
+        <v>877</v>
       </c>
       <c r="S34" t="s">
         <v>728</v>
@@ -13625,11 +13751,11 @@
       </c>
       <c r="O35"/>
       <c r="P35" t="s">
-        <v>199</v>
+        <v>839</v>
       </c>
       <c r="Q35"/>
       <c r="R35" t="s">
-        <v>199</v>
+        <v>839</v>
       </c>
       <c r="S35" t="s">
         <v>47</v>
@@ -13687,11 +13813,11 @@
       </c>
       <c r="O36"/>
       <c r="P36" t="s">
-        <v>95</v>
+        <v>864</v>
       </c>
       <c r="Q36"/>
       <c r="R36" t="s">
-        <v>95</v>
+        <v>864</v>
       </c>
       <c r="S36" t="s">
         <v>729</v>
@@ -13821,11 +13947,11 @@
       </c>
       <c r="O38"/>
       <c r="P38" t="s">
-        <v>691</v>
+        <v>878</v>
       </c>
       <c r="Q38"/>
       <c r="R38" t="s">
-        <v>691</v>
+        <v>878</v>
       </c>
       <c r="S38" t="s">
         <v>796</v>
@@ -13897,11 +14023,11 @@
       </c>
       <c r="O39"/>
       <c r="P39" t="s">
-        <v>692</v>
+        <v>879</v>
       </c>
       <c r="Q39"/>
       <c r="R39" t="s">
-        <v>692</v>
+        <v>879</v>
       </c>
       <c r="S39" t="s">
         <v>176</v>
@@ -13975,11 +14101,11 @@
       </c>
       <c r="O40"/>
       <c r="P40" t="s">
-        <v>693</v>
+        <v>880</v>
       </c>
       <c r="Q40"/>
       <c r="R40" t="s">
-        <v>693</v>
+        <v>880</v>
       </c>
       <c r="S40" t="s">
         <v>797</v>
@@ -14045,11 +14171,11 @@
       </c>
       <c r="O41"/>
       <c r="P41" t="s">
-        <v>199</v>
+        <v>839</v>
       </c>
       <c r="Q41"/>
       <c r="R41" t="s">
-        <v>199</v>
+        <v>839</v>
       </c>
       <c r="S41" t="s">
         <v>789</v>
@@ -14107,11 +14233,11 @@
       </c>
       <c r="O42"/>
       <c r="P42" t="s">
-        <v>208</v>
+        <v>881</v>
       </c>
       <c r="Q42"/>
       <c r="R42" t="s">
-        <v>208</v>
+        <v>881</v>
       </c>
       <c r="S42" t="s">
         <v>798</v>
@@ -14293,11 +14419,11 @@
       </c>
       <c r="O45"/>
       <c r="P45" t="s">
-        <v>694</v>
+        <v>882</v>
       </c>
       <c r="Q45"/>
       <c r="R45" t="s">
-        <v>694</v>
+        <v>882</v>
       </c>
       <c r="S45" t="s">
         <v>491</v>
@@ -14445,11 +14571,11 @@
       </c>
       <c r="O47"/>
       <c r="P47" t="s">
-        <v>695</v>
+        <v>883</v>
       </c>
       <c r="Q47"/>
       <c r="R47" t="s">
-        <v>695</v>
+        <v>883</v>
       </c>
       <c r="S47" t="s">
         <v>259</v>
@@ -14659,11 +14785,11 @@
       </c>
       <c r="O50"/>
       <c r="P50" t="s">
-        <v>696</v>
+        <v>884</v>
       </c>
       <c r="Q50"/>
       <c r="R50" t="s">
-        <v>696</v>
+        <v>884</v>
       </c>
       <c r="S50" t="s">
         <v>735</v>
@@ -14719,11 +14845,11 @@
       <c r="N51"/>
       <c r="O51"/>
       <c r="P51" t="s">
-        <v>697</v>
+        <v>885</v>
       </c>
       <c r="Q51"/>
       <c r="R51" t="s">
-        <v>697</v>
+        <v>885</v>
       </c>
       <c r="S51" t="s">
         <v>335</v>
@@ -14795,11 +14921,11 @@
       </c>
       <c r="O52"/>
       <c r="P52" t="s">
-        <v>698</v>
+        <v>886</v>
       </c>
       <c r="Q52"/>
       <c r="R52" t="s">
-        <v>698</v>
+        <v>886</v>
       </c>
       <c r="S52" t="s">
         <v>736</v>
@@ -14877,11 +15003,11 @@
       </c>
       <c r="O53"/>
       <c r="P53" t="s">
-        <v>350</v>
+        <v>887</v>
       </c>
       <c r="Q53"/>
       <c r="R53" t="s">
-        <v>350</v>
+        <v>887</v>
       </c>
       <c r="S53" t="s">
         <v>737</v>
@@ -14947,11 +15073,11 @@
       <c r="N54"/>
       <c r="O54"/>
       <c r="P54" t="s">
-        <v>699</v>
+        <v>888</v>
       </c>
       <c r="Q54"/>
       <c r="R54" t="s">
-        <v>699</v>
+        <v>888</v>
       </c>
       <c r="S54" t="s">
         <v>801</v>
@@ -15079,11 +15205,11 @@
       </c>
       <c r="O56"/>
       <c r="P56" t="s">
-        <v>700</v>
+        <v>889</v>
       </c>
       <c r="Q56"/>
       <c r="R56" t="s">
-        <v>700</v>
+        <v>889</v>
       </c>
       <c r="S56" t="s">
         <v>739</v>
@@ -15133,11 +15259,11 @@
       <c r="N57"/>
       <c r="O57"/>
       <c r="P57" t="s">
-        <v>701</v>
+        <v>890</v>
       </c>
       <c r="Q57"/>
       <c r="R57" t="s">
-        <v>701</v>
+        <v>890</v>
       </c>
       <c r="S57" t="s">
         <v>802</v>
@@ -15241,11 +15367,11 @@
       </c>
       <c r="O59"/>
       <c r="P59" t="s">
-        <v>702</v>
+        <v>891</v>
       </c>
       <c r="Q59"/>
       <c r="R59" t="s">
-        <v>702</v>
+        <v>891</v>
       </c>
       <c r="S59" t="s">
         <v>742</v>

</xml_diff>